<commit_message>
adding simple time estimation
</commit_message>
<xml_diff>
--- a/playoffs-example-medium.xlsx
+++ b/playoffs-example-medium.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="21580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="Elimination Matches" sheetId="7" r:id="rId4"/>
-    <sheet name="Names to Print" sheetId="8" r:id="rId5"/>
-    <sheet name="Tree 1" sheetId="9" r:id="rId12"/>
-    <sheet name="Tree 2" sheetId="10" r:id="rId13"/>
+    <sheet name="Time Estimator" sheetId="9" r:id="rId2"/>
+    <sheet name="Elimination Matches" sheetId="7" r:id="rId5"/>
+    <sheet name="Names to Print" sheetId="8" r:id="rId6"/>
+    <sheet name="Tree 1" sheetId="10" r:id="rId13"/>
+    <sheet name="Tree 2" sheetId="11" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="115">
   <si>
     <t>Elimination Round 1</t>
   </si>
@@ -48,6 +49,33 @@
     <t>Tournament Pools</t>
   </si>
   <si>
+    <t>Number of pools</t>
+  </si>
+  <si>
+    <t>Team size</t>
+  </si>
+  <si>
+    <t>Matches per pool</t>
+  </si>
+  <si>
+    <t>Time per match</t>
+  </si>
+  <si>
+    <t>Total time for matches</t>
+  </si>
+  <si>
+    <t>Padding time for rotation</t>
+  </si>
+  <si>
+    <t>Time for breaks</t>
+  </si>
+  <si>
+    <t>Total Time</t>
+  </si>
+  <si>
+    <t>Number of Elimination Matches</t>
+  </si>
+  <si>
     <t>Number</t>
   </si>
   <si>
@@ -60,6 +88,132 @@
     <t>Display Name</t>
   </si>
   <si>
+    <t>Ygritte</t>
+  </si>
+  <si>
+    <t>Team Alpha</t>
+  </si>
+  <si>
+    <t>Y. YGRITTE</t>
+  </si>
+  <si>
+    <t>Tyrion Lannister</t>
+  </si>
+  <si>
+    <t>Team Upsilon</t>
+  </si>
+  <si>
+    <t>T. LANNISTER</t>
+  </si>
+  <si>
+    <t>Xaro Xhoan Daxos</t>
+  </si>
+  <si>
+    <t>Team Omega</t>
+  </si>
+  <si>
+    <t>X. DAXOS</t>
+  </si>
+  <si>
+    <t>Ulysses</t>
+  </si>
+  <si>
+    <t>Team Phi</t>
+  </si>
+  <si>
+    <t>U. ULYSSES</t>
+  </si>
+  <si>
+    <t>Jon Snow</t>
+  </si>
+  <si>
+    <t>Team Kappa</t>
+  </si>
+  <si>
+    <t>J. SNOW</t>
+  </si>
+  <si>
+    <t>Frodo Baggins</t>
+  </si>
+  <si>
+    <t>Team Zeta</t>
+  </si>
+  <si>
+    <t>F. BAGGINS</t>
+  </si>
+  <si>
+    <t>Eddard Stark</t>
+  </si>
+  <si>
+    <t>Team Epsilon</t>
+  </si>
+  <si>
+    <t>E. STARK</t>
+  </si>
+  <si>
+    <t>Othello</t>
+  </si>
+  <si>
+    <t>Team Omicron</t>
+  </si>
+  <si>
+    <t>O. OTHELLO</t>
+  </si>
+  <si>
+    <t>Daenerys Targaryen</t>
+  </si>
+  <si>
+    <t>Team Delta</t>
+  </si>
+  <si>
+    <t>D. TARGARYEN</t>
+  </si>
+  <si>
+    <t>Cersei Lannister</t>
+  </si>
+  <si>
+    <t>Team Gamma</t>
+  </si>
+  <si>
+    <t>C. LANNISTER</t>
+  </si>
+  <si>
+    <t>Ron Weasley</t>
+  </si>
+  <si>
+    <t>Team Sigma</t>
+  </si>
+  <si>
+    <t>R. WEASLEY</t>
+  </si>
+  <si>
+    <t>Inigo Montoya</t>
+  </si>
+  <si>
+    <t>Team Iota</t>
+  </si>
+  <si>
+    <t>I. MONTOYA</t>
+  </si>
+  <si>
+    <t>Quirinus Quirrell</t>
+  </si>
+  <si>
+    <t>Team Rho</t>
+  </si>
+  <si>
+    <t>Q. QUIRRELL</t>
+  </si>
+  <si>
+    <t>Willy Wonka</t>
+  </si>
+  <si>
+    <t>Team Psi</t>
+  </si>
+  <si>
+    <t>W. WONKA</t>
+  </si>
+  <si>
     <t>Moby Dick</t>
   </si>
   <si>
@@ -78,13 +232,13 @@
     <t>K. EVERDEEN</t>
   </si>
   <si>
-    <t>Quirinus Quirrell</t>
-  </si>
-  <si>
-    <t>Team Rho</t>
-  </si>
-  <si>
-    <t>Q. QUIRRELL</t>
+    <t>Samwise Gamgee</t>
+  </si>
+  <si>
+    <t>Team Tau</t>
+  </si>
+  <si>
+    <t>S. GAMGEE</t>
   </si>
   <si>
     <t>Neville Longbottom</t>
@@ -96,13 +250,22 @@
     <t>N. LONGBOTTOM</t>
   </si>
   <si>
-    <t>Inigo Montoya</t>
-  </si>
-  <si>
-    <t>Team Iota</t>
-  </si>
-  <si>
-    <t>I. MONTOYA</t>
+    <t>Legolas Greenleaf</t>
+  </si>
+  <si>
+    <t>Team Mu</t>
+  </si>
+  <si>
+    <t>L. GREENLEAF</t>
+  </si>
+  <si>
+    <t>Petyr Baelish</t>
+  </si>
+  <si>
+    <t>Team Pi</t>
+  </si>
+  <si>
+    <t>P. BAELISH</t>
   </si>
   <si>
     <t>Gandalf The Grey</t>
@@ -114,42 +277,6 @@
     <t>G. GREY</t>
   </si>
   <si>
-    <t>Petyr Baelish</t>
-  </si>
-  <si>
-    <t>Team Pi</t>
-  </si>
-  <si>
-    <t>P. BAELISH</t>
-  </si>
-  <si>
-    <t>Cersei Lannister</t>
-  </si>
-  <si>
-    <t>Team Gamma</t>
-  </si>
-  <si>
-    <t>C. LANNISTER</t>
-  </si>
-  <si>
-    <t>Willy Wonka</t>
-  </si>
-  <si>
-    <t>Team Psi</t>
-  </si>
-  <si>
-    <t>W. WONKA</t>
-  </si>
-  <si>
-    <t>Ulysses</t>
-  </si>
-  <si>
-    <t>Team Phi</t>
-  </si>
-  <si>
-    <t>U. ULYSSES</t>
-  </si>
-  <si>
     <t>Voldemort</t>
   </si>
   <si>
@@ -159,33 +286,6 @@
     <t>V. VOLDEMORT</t>
   </si>
   <si>
-    <t>Frodo Baggins</t>
-  </si>
-  <si>
-    <t>Team Zeta</t>
-  </si>
-  <si>
-    <t>F. BAGGINS</t>
-  </si>
-  <si>
-    <t>Eddard Stark</t>
-  </si>
-  <si>
-    <t>Team Epsilon</t>
-  </si>
-  <si>
-    <t>E. STARK</t>
-  </si>
-  <si>
-    <t>Daenerys Targaryen</t>
-  </si>
-  <si>
-    <t>Team Delta</t>
-  </si>
-  <si>
-    <t>D. TARGARYEN</t>
-  </si>
-  <si>
     <t>Hermione Granger</t>
   </si>
   <si>
@@ -193,78 +293,6 @@
   </si>
   <si>
     <t>H. GRANGER</t>
-  </si>
-  <si>
-    <t>Ron Weasley</t>
-  </si>
-  <si>
-    <t>Team Sigma</t>
-  </si>
-  <si>
-    <t>R. WEASLEY</t>
-  </si>
-  <si>
-    <t>Ygritte</t>
-  </si>
-  <si>
-    <t>Team Alpha</t>
-  </si>
-  <si>
-    <t>Y. YGRITTE</t>
-  </si>
-  <si>
-    <t>Tyrion Lannister</t>
-  </si>
-  <si>
-    <t>Team Upsilon</t>
-  </si>
-  <si>
-    <t>T. LANNISTER</t>
-  </si>
-  <si>
-    <t>Jon Snow</t>
-  </si>
-  <si>
-    <t>Team Kappa</t>
-  </si>
-  <si>
-    <t>J. SNOW</t>
-  </si>
-  <si>
-    <t>Legolas Greenleaf</t>
-  </si>
-  <si>
-    <t>Team Mu</t>
-  </si>
-  <si>
-    <t>L. GREENLEAF</t>
-  </si>
-  <si>
-    <t>Xaro Xhoan Daxos</t>
-  </si>
-  <si>
-    <t>Team Omega</t>
-  </si>
-  <si>
-    <t>X. DAXOS</t>
-  </si>
-  <si>
-    <t>Samwise Gamgee</t>
-  </si>
-  <si>
-    <t>Team Tau</t>
-  </si>
-  <si>
-    <t>S. GAMGEE</t>
-  </si>
-  <si>
-    <t>Othello</t>
-  </si>
-  <si>
-    <t>Team Omicron</t>
-  </si>
-  <si>
-    <t>O. OTHELLO</t>
   </si>
   <si>
     <t>Match 1</t>
@@ -364,6 +392,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="16">
     <font>
       <sz val="10"/>
@@ -614,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -635,6 +666,18 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -959,7 +1002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
@@ -972,16 +1015,16 @@
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" customHeight="true">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="12.75" customHeight="true">
@@ -989,13 +1032,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12.75" customHeight="true">
@@ -1003,13 +1046,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="true">
@@ -1017,13 +1060,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12.75" customHeight="true">
@@ -1031,13 +1074,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12.75" customHeight="true">
@@ -1045,13 +1088,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12.75" customHeight="true">
@@ -1059,13 +1102,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12.75" customHeight="true">
@@ -1073,13 +1116,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12.75" customHeight="true">
@@ -1087,13 +1130,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12.75" customHeight="true">
@@ -1101,13 +1144,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12.75" customHeight="true">
@@ -1115,13 +1158,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12.75" customHeight="true">
@@ -1129,13 +1172,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12.75" customHeight="true">
@@ -1143,13 +1186,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12.75" customHeight="true">
@@ -1157,13 +1200,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="12.75" customHeight="true">
@@ -1171,13 +1214,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12.75" customHeight="true">
@@ -1185,13 +1228,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.75" customHeight="true">
@@ -1199,13 +1242,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12.75" customHeight="true">
@@ -1213,13 +1256,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12.75" customHeight="true">
@@ -1227,13 +1270,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12.75" customHeight="true">
@@ -1241,13 +1284,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="12.75" customHeight="true">
@@ -1255,13 +1298,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12.75" customHeight="true">
@@ -1269,13 +1312,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="12.75" customHeight="true">
@@ -1283,13 +1326,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="12.75" customHeight="true">
@@ -1297,13 +1340,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="12.75" customHeight="true"/>
@@ -2358,309 +2401,640 @@
   </cols>
   <sheetData>
     <row r="6">
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="E7" s="24"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="20"/>
+    </row>
+    <row r="8">
+      <c r="G8" s="20"/>
+    </row>
+    <row r="9">
+      <c r="G9" s="20"/>
+    </row>
+    <row r="10">
+      <c r="G10" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="G11" s="20"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="20"/>
+    </row>
+    <row r="12">
+      <c r="G12" s="20"/>
+      <c r="I12" s="20"/>
+    </row>
+    <row r="13">
+      <c r="E13" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="23"/>
+      <c r="G13" s="20"/>
+      <c r="I13" s="20"/>
+    </row>
+    <row r="14">
+      <c r="E14" s="24"/>
+      <c r="I14" s="20"/>
+    </row>
+    <row r="15">
+      <c r="I15" s="20"/>
+    </row>
+    <row r="16">
+      <c r="I16" s="20"/>
+    </row>
+    <row r="17">
+      <c r="I17" s="20"/>
+    </row>
+    <row r="18">
+      <c r="I18" s="21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="I19" s="20"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="20"/>
+    </row>
+    <row r="20">
+      <c r="I20" s="20"/>
+      <c r="K20" s="20"/>
+    </row>
+    <row r="21">
+      <c r="E21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="20"/>
+      <c r="K21" s="20"/>
+    </row>
+    <row r="22">
+      <c r="E22" s="24"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="K22" s="20"/>
+    </row>
+    <row r="23">
+      <c r="G23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="K23" s="20"/>
+    </row>
+    <row r="24">
+      <c r="G24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="K24" s="20"/>
+    </row>
+    <row r="25">
+      <c r="G25" s="21">
+        <v>9</v>
+      </c>
+      <c r="H25" s="23"/>
+      <c r="I25" s="20"/>
+      <c r="K25" s="20"/>
+    </row>
+    <row r="26">
+      <c r="C26" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="20"/>
+      <c r="K26" s="20"/>
+    </row>
+    <row r="27">
+      <c r="C27" s="24"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="K27" s="20"/>
+    </row>
+    <row r="28">
+      <c r="E28" s="21">
+        <v>1</v>
+      </c>
+      <c r="F28" s="23"/>
+      <c r="G28" s="20"/>
+      <c r="K28" s="20"/>
+    </row>
+    <row r="29">
+      <c r="C29" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="23"/>
+      <c r="E29" s="20"/>
+      <c r="K29" s="20"/>
+    </row>
+    <row r="30">
+      <c r="C30" s="24"/>
+      <c r="K30" s="20"/>
+    </row>
+    <row r="31">
+      <c r="K31" s="20"/>
+    </row>
+    <row r="32">
+      <c r="K32" s="20"/>
+    </row>
+    <row r="33">
+      <c r="K33" s="20"/>
+    </row>
+    <row r="34">
+      <c r="K34" s="21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="K35" s="20"/>
+    </row>
+    <row r="36">
+      <c r="K36" s="20"/>
+    </row>
+    <row r="37">
+      <c r="E37" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="K37" s="20"/>
+    </row>
+    <row r="38">
+      <c r="E38" s="24"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="20"/>
+      <c r="K38" s="20"/>
+    </row>
+    <row r="39">
+      <c r="G39" s="20"/>
+      <c r="K39" s="20"/>
+    </row>
+    <row r="40">
+      <c r="G40" s="20"/>
+      <c r="K40" s="20"/>
+    </row>
+    <row r="41">
+      <c r="G41" s="21">
+        <v>10</v>
+      </c>
+      <c r="K41" s="20"/>
+    </row>
+    <row r="42">
+      <c r="C42" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G42" s="20"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="20"/>
+      <c r="K42" s="20"/>
+    </row>
+    <row r="43">
+      <c r="C43" s="24"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="K43" s="20"/>
+    </row>
+    <row r="44">
+      <c r="E44" s="21">
+        <v>2</v>
+      </c>
+      <c r="F44" s="23"/>
+      <c r="G44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="K44" s="20"/>
+    </row>
+    <row r="45">
+      <c r="C45" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" s="23"/>
+      <c r="E45" s="20"/>
+      <c r="I45" s="20"/>
+      <c r="K45" s="20"/>
+    </row>
+    <row r="46">
+      <c r="C46" s="24"/>
+      <c r="I46" s="20"/>
+      <c r="K46" s="20"/>
+    </row>
+    <row r="47">
+      <c r="I47" s="20"/>
+      <c r="K47" s="20"/>
+    </row>
+    <row r="48">
+      <c r="I48" s="20"/>
+      <c r="K48" s="20"/>
+    </row>
+    <row r="49">
+      <c r="I49" s="21">
+        <v>17</v>
+      </c>
+      <c r="J49" s="23"/>
+      <c r="K49" s="20"/>
+    </row>
+    <row r="50">
+      <c r="I50" s="20"/>
+    </row>
+    <row r="51">
+      <c r="I51" s="20"/>
+    </row>
+    <row r="52">
+      <c r="E52" s="24" t="s">
         <v>41</v>
       </c>
+      <c r="I52" s="20"/>
+    </row>
+    <row r="53">
+      <c r="E53" s="24"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="20"/>
+      <c r="I53" s="20"/>
+    </row>
+    <row r="54">
+      <c r="G54" s="20"/>
+      <c r="I54" s="20"/>
+    </row>
+    <row r="55">
+      <c r="G55" s="20"/>
+      <c r="I55" s="20"/>
+    </row>
+    <row r="56">
+      <c r="G56" s="21">
+        <v>11</v>
+      </c>
+      <c r="H56" s="23"/>
+      <c r="I56" s="20"/>
+    </row>
+    <row r="57">
+      <c r="C57" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G57" s="20"/>
+    </row>
+    <row r="58">
+      <c r="C58" s="24"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="20"/>
+      <c r="G58" s="20"/>
+    </row>
+    <row r="59">
+      <c r="E59" s="21">
+        <v>3</v>
+      </c>
+      <c r="F59" s="23"/>
+      <c r="G59" s="20"/>
+    </row>
+    <row r="60">
+      <c r="C60" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D60" s="23"/>
+      <c r="E60" s="20"/>
+    </row>
+    <row r="61">
+      <c r="C61" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="C60:C61"/>
+  </mergeCells>
+  <printOptions horizontalCentered="true" verticalCentered="true"/>
+  <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4065E12-1BC4-BF48-9DCD-AFB9407081DC}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="true"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="false" view="pageLayout" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P56" sqref="P56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="13"/>
+  <cols>
+    <col customWidth="true" max="1" min="1" width="20.83203125"/>
+    <col customWidth="true" max="3" min="3" width="20"/>
+    <col customWidth="true" max="5" min="5" width="20"/>
+  </cols>
+  <sheetData>
+    <row r="6">
+      <c r="E6" s="24" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7">
-      <c r="E7" s="20"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="16"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="20"/>
     </row>
     <row r="8">
-      <c r="G8" s="16"/>
+      <c r="G8" s="20"/>
     </row>
     <row r="9">
-      <c r="G9" s="16"/>
+      <c r="G9" s="20"/>
     </row>
     <row r="10">
-      <c r="G10" s="17">
+      <c r="G10" s="21">
         <v>12</v>
       </c>
     </row>
     <row r="11">
-      <c r="C11" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="16"/>
+      <c r="C11" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="20"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="20"/>
     </row>
     <row r="12">
-      <c r="C12" s="20"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="I12" s="16"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="I12" s="20"/>
     </row>
     <row r="13">
-      <c r="E13" s="17">
+      <c r="E13" s="21">
         <v>4</v>
       </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="16"/>
-      <c r="I13" s="16"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="20"/>
+      <c r="I13" s="20"/>
     </row>
     <row r="14">
-      <c r="C14" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="16"/>
-      <c r="I14" s="16"/>
+      <c r="C14" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="20"/>
+      <c r="I14" s="20"/>
     </row>
     <row r="15">
-      <c r="C15" s="20"/>
-      <c r="I15" s="16"/>
+      <c r="C15" s="24"/>
+      <c r="I15" s="20"/>
     </row>
     <row r="16">
-      <c r="I16" s="16"/>
+      <c r="I16" s="20"/>
     </row>
     <row r="17">
-      <c r="I17" s="16"/>
+      <c r="I17" s="20"/>
     </row>
     <row r="18">
-      <c r="I18" s="17">
+      <c r="I18" s="21">
         <v>18</v>
       </c>
     </row>
     <row r="19">
-      <c r="I19" s="16"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="16"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="20"/>
     </row>
     <row r="20">
-      <c r="I20" s="16"/>
-      <c r="K20" s="16"/>
+      <c r="I20" s="20"/>
+      <c r="K20" s="20"/>
     </row>
     <row r="21">
-      <c r="E21" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="I21" s="16"/>
-      <c r="K21" s="16"/>
+      <c r="E21" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="20"/>
+      <c r="K21" s="20"/>
     </row>
     <row r="22">
-      <c r="E22" s="20"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="K22" s="16"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="K22" s="20"/>
     </row>
     <row r="23">
-      <c r="G23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="K23" s="16"/>
+      <c r="G23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="K23" s="20"/>
     </row>
     <row r="24">
-      <c r="G24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="K24" s="16"/>
+      <c r="G24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="K24" s="20"/>
     </row>
     <row r="25">
-      <c r="G25" s="17">
+      <c r="G25" s="21">
         <v>13</v>
       </c>
-      <c r="H25" s="19"/>
-      <c r="I25" s="16"/>
-      <c r="K25" s="16"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="20"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26">
-      <c r="C26" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="G26" s="16"/>
-      <c r="K26" s="16"/>
+      <c r="C26" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" s="20"/>
+      <c r="K26" s="20"/>
     </row>
     <row r="27">
-      <c r="C27" s="20"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="K27" s="16"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="K27" s="20"/>
     </row>
     <row r="28">
-      <c r="E28" s="17">
+      <c r="E28" s="21">
         <v>5</v>
       </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="16"/>
-      <c r="K28" s="16"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="20"/>
+      <c r="K28" s="20"/>
     </row>
     <row r="29">
-      <c r="C29" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="16"/>
-      <c r="K29" s="16"/>
+      <c r="C29" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="23"/>
+      <c r="E29" s="20"/>
+      <c r="K29" s="20"/>
     </row>
     <row r="30">
-      <c r="C30" s="20"/>
-      <c r="K30" s="16"/>
+      <c r="C30" s="24"/>
+      <c r="K30" s="20"/>
     </row>
     <row r="31">
-      <c r="K31" s="16"/>
+      <c r="K31" s="20"/>
     </row>
     <row r="32">
-      <c r="K32" s="16"/>
+      <c r="K32" s="20"/>
     </row>
     <row r="33">
-      <c r="K33" s="16"/>
+      <c r="K33" s="20"/>
     </row>
     <row r="34">
-      <c r="K34" s="17">
+      <c r="K34" s="21">
         <v>21</v>
       </c>
     </row>
     <row r="35">
-      <c r="K35" s="16"/>
+      <c r="K35" s="20"/>
     </row>
     <row r="36">
-      <c r="K36" s="16"/>
+      <c r="K36" s="20"/>
     </row>
     <row r="37">
-      <c r="E37" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="K37" s="16"/>
+      <c r="E37" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="K37" s="20"/>
     </row>
     <row r="38">
-      <c r="E38" s="20"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="16"/>
-      <c r="K38" s="16"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="20"/>
+      <c r="K38" s="20"/>
     </row>
     <row r="39">
-      <c r="G39" s="16"/>
-      <c r="K39" s="16"/>
+      <c r="G39" s="20"/>
+      <c r="K39" s="20"/>
     </row>
     <row r="40">
-      <c r="G40" s="16"/>
-      <c r="K40" s="16"/>
+      <c r="G40" s="20"/>
+      <c r="K40" s="20"/>
     </row>
     <row r="41">
-      <c r="G41" s="17">
+      <c r="G41" s="21">
         <v>14</v>
       </c>
-      <c r="K41" s="16"/>
+      <c r="K41" s="20"/>
     </row>
     <row r="42">
-      <c r="C42" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="G42" s="16"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="16"/>
-      <c r="K42" s="16"/>
+      <c r="C42" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="G42" s="20"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="20"/>
+      <c r="K42" s="20"/>
     </row>
     <row r="43">
-      <c r="C43" s="20"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="I43" s="16"/>
-      <c r="K43" s="16"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="K43" s="20"/>
     </row>
     <row r="44">
-      <c r="E44" s="17">
+      <c r="E44" s="21">
         <v>6</v>
       </c>
-      <c r="F44" s="19"/>
-      <c r="G44" s="16"/>
-      <c r="I44" s="16"/>
-      <c r="K44" s="16"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="K44" s="20"/>
     </row>
     <row r="45">
-      <c r="C45" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="16"/>
-      <c r="I45" s="16"/>
-      <c r="K45" s="16"/>
+      <c r="C45" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45" s="23"/>
+      <c r="E45" s="20"/>
+      <c r="I45" s="20"/>
+      <c r="K45" s="20"/>
     </row>
     <row r="46">
-      <c r="C46" s="20"/>
-      <c r="I46" s="16"/>
-      <c r="K46" s="16"/>
+      <c r="C46" s="24"/>
+      <c r="I46" s="20"/>
+      <c r="K46" s="20"/>
     </row>
     <row r="47">
-      <c r="I47" s="16"/>
-      <c r="K47" s="16"/>
+      <c r="I47" s="20"/>
+      <c r="K47" s="20"/>
     </row>
     <row r="48">
-      <c r="I48" s="16"/>
-      <c r="K48" s="16"/>
+      <c r="I48" s="20"/>
+      <c r="K48" s="20"/>
     </row>
     <row r="49">
-      <c r="I49" s="17">
+      <c r="I49" s="21">
         <v>19</v>
       </c>
-      <c r="J49" s="19"/>
-      <c r="K49" s="16"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="20"/>
     </row>
     <row r="50">
-      <c r="I50" s="16"/>
+      <c r="I50" s="20"/>
     </row>
     <row r="51">
-      <c r="I51" s="16"/>
+      <c r="I51" s="20"/>
     </row>
     <row r="52">
-      <c r="E52" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="I52" s="16"/>
+      <c r="E52" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="I52" s="20"/>
     </row>
     <row r="53">
-      <c r="E53" s="20"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="16"/>
-      <c r="I53" s="16"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="20"/>
+      <c r="I53" s="20"/>
     </row>
     <row r="54">
-      <c r="G54" s="16"/>
-      <c r="I54" s="16"/>
+      <c r="G54" s="20"/>
+      <c r="I54" s="20"/>
     </row>
     <row r="55">
-      <c r="G55" s="16"/>
-      <c r="I55" s="16"/>
+      <c r="G55" s="20"/>
+      <c r="I55" s="20"/>
     </row>
     <row r="56">
-      <c r="G56" s="17">
+      <c r="G56" s="21">
         <v>15</v>
       </c>
-      <c r="H56" s="19"/>
-      <c r="I56" s="16"/>
+      <c r="H56" s="23"/>
+      <c r="I56" s="20"/>
     </row>
     <row r="57">
-      <c r="C57" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="G57" s="16"/>
+      <c r="C57" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="G57" s="20"/>
     </row>
     <row r="58">
-      <c r="C58" s="20"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="16"/>
-      <c r="G58" s="16"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="20"/>
+      <c r="G58" s="20"/>
     </row>
     <row r="59">
-      <c r="E59" s="17">
+      <c r="E59" s="21">
         <v>7</v>
       </c>
-      <c r="F59" s="19"/>
-      <c r="G59" s="16"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="20"/>
     </row>
     <row r="60">
-      <c r="C60" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="D60" s="19"/>
-      <c r="E60" s="16"/>
+      <c r="C60" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D60" s="23"/>
+      <c r="E60" s="20"/>
     </row>
     <row r="61">
-      <c r="C61" s="20"/>
+      <c r="C61" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2682,7 +3056,219 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{176316AF-4790-BF4E-A6AB-8C7837CD465B}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col customWidth="true" max="1" min="1" width="21.83203125"/>
+    <col customWidth="true" max="4" min="4" width="14.6640625"/>
+    <col customWidth="true" max="5" min="5" width="17"/>
+    <col customWidth="true" max="7" min="6" width="13.1640625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="51">
+      <c r="A1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="11" customFormat="true" ht="16">
+      <c r="A2" s="11">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0</v>
+      </c>
+      <c r="C2" s="11">
+        <v>0</v>
+      </c>
+      <c r="D2" s="12">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="E2" s="12">
+        <f>(A2*B2*C2*D2)</f>
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="F2" s="12">
+        <v>3.4722222222222224E-4</v>
+      </c>
+      <c r="G2" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H2" s="12">
+        <f>E2+(A2*C2*F2)+G2</f>
+        <v>6.041666666666666E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16">
+      <c r="A3" s="11">
+        <v>0</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="E3" s="12">
+        <f>(A3*B3*C3*D3)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="12">
+        <v>3.4722222222222224E-4</v>
+      </c>
+      <c r="G3" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H3" s="12">
+        <f>E3+(A3*C3*F3)+G3</f>
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" ht="16">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+    </row>
+    <row r="6" spans="1:8" ht="16">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="1:8" ht="51">
+      <c r="A7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="11" customFormat="true" ht="16">
+      <c r="A8" s="11">
+        <v>22</v>
+      </c>
+      <c r="B8" s="11">
+        <v>0</v>
+      </c>
+      <c r="D8" s="12">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="E8" s="12">
+        <f>(A8*B8*D8)</f>
+        <v>4.1666666666666671E-2</v>
+      </c>
+      <c r="F8" s="12">
+        <v>3.4722222222222224E-4</v>
+      </c>
+      <c r="G8" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H8" s="12">
+        <f>E8+(A8*F8)+G8</f>
+        <v>6.4236111111111119E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" ht="16">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" ht="16">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D4E4C4-15C1-724B-94C9-DD9C94F4D3CF}">
   <dimension ref="A1:O1"/>
   <sheetViews>
@@ -2707,1033 +3293,1033 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="true">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
     </row>
     <row r="3">
-      <c r="A3" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="I3" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
+      <c r="A3" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="I3" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
     </row>
     <row r="4">
-      <c r="A4" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="L4" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="O4" s="26" t="s">
-        <v>78</v>
+      <c r="A4" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="L4" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="O4" s="30" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="24" t="str">
+      <c r="A5" s="28" t="str">
         <f>'data'!B5</f>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24" t="str">
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28" t="str">
         <f>'data'!B6</f>
       </c>
-      <c r="I5" s="24" t="str">
+      <c r="I5" s="28" t="str">
         <f>'data'!B8</f>
       </c>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24" t="str">
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28" t="str">
         <f>'data'!B9</f>
       </c>
     </row>
     <row r="7">
       <c r="F7" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="G7" s="23"/>
       <c r="N7" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="O7" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="O7" s="23"/>
     </row>
     <row r="8">
       <c r="F8" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G8" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="G8" s="23"/>
       <c r="N8" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="O8" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="O8" s="23"/>
     </row>
     <row r="11">
-      <c r="A11" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="I11" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
+      <c r="A11" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="I11" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
     </row>
     <row r="12">
-      <c r="A12" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G12" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="I12" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="O12" s="28" t="s">
-        <v>78</v>
+      <c r="A12" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="L12" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="O12" s="32" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="24" t="str">
+      <c r="A13" s="28" t="str">
         <f>'data'!B11</f>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24" t="str">
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28" t="str">
         <f>'data'!B12</f>
       </c>
-      <c r="I13" s="24" t="str">
+      <c r="I13" s="28" t="str">
         <f>'data'!B14</f>
       </c>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24" t="str">
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28" t="str">
         <f>'data'!B15</f>
       </c>
     </row>
     <row r="15">
       <c r="F15" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="G15" s="23"/>
       <c r="N15" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="O15" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="O15" s="23"/>
     </row>
     <row r="16">
       <c r="F16" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G16" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="G16" s="23"/>
       <c r="N16" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="O16" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="O16" s="23"/>
     </row>
     <row r="19">
-      <c r="A19" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="I19" s="20" t="s">
+      <c r="A19" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="I19" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G20" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="I20" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="L20" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="O20" s="30" t="s">
-        <v>78</v>
+      <c r="D20" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="L20" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="O20" s="34" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="24" t="str">
+      <c r="A21" s="28" t="str">
         <f>'data'!B17</f>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24" t="str">
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28" t="str">
         <f>'data'!B18</f>
       </c>
-      <c r="I21" s="24" t="str">
+      <c r="I21" s="28" t="str">
         <f>'data'!B20</f>
       </c>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24" t="str">
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28" t="str">
         <f>'data'!B21</f>
       </c>
     </row>
     <row r="23">
       <c r="F23" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G23" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="G23" s="23"/>
       <c r="N23" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="O23" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="O23" s="23"/>
     </row>
     <row r="24">
       <c r="F24" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G24" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="G24" s="23"/>
       <c r="N24" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="O24" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="O24" s="23"/>
     </row>
     <row r="27">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G28" s="31" t="s">
-        <v>78</v>
+      <c r="G28" s="35" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="24" t="str">
+      <c r="A29" s="28" t="str">
         <f>'data'!B23</f>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24" t="str">
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28" t="str">
         <f>'data'!B24</f>
       </c>
     </row>
     <row r="31">
       <c r="F31" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G31" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="G31" s="23"/>
     </row>
     <row r="32">
       <c r="F32" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G32" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="G32" s="23"/>
     </row>
     <row r="40">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="24"/>
+      <c r="L40" s="24"/>
+      <c r="M40" s="24"/>
+      <c r="N40" s="24"/>
+      <c r="O40" s="24"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="I42" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="J42" s="24"/>
+      <c r="K42" s="24"/>
+      <c r="L42" s="24"/>
+      <c r="M42" s="24"/>
+      <c r="N42" s="24"/>
+      <c r="O42" s="24"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G43" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="20"/>
-      <c r="M40" s="20"/>
-      <c r="N40" s="20"/>
-      <c r="O40" s="20"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="I42" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="20"/>
-      <c r="N42" s="20"/>
-      <c r="O42" s="20"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D43" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G43" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="I43" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="L43" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="O43" s="33" t="s">
-        <v>78</v>
+      <c r="I43" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="L43" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="O43" s="37" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="24" t="str">
+      <c r="A44" s="28" t="str">
         <f>'data'!B2</f>
       </c>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24" t="str">
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28" t="str">
         <f>'data'!B3</f>
       </c>
-      <c r="I44" s="24" t="str">
+      <c r="I44" s="28" t="str">
         <f>'data'!B4</f>
       </c>
-      <c r="J44" s="24"/>
-      <c r="K44" s="24"/>
-      <c r="L44" s="24"/>
-      <c r="M44" s="24"/>
-      <c r="N44" s="24"/>
-      <c r="O44" s="24" t="str">
+      <c r="J44" s="28"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="28"/>
+      <c r="N44" s="28"/>
+      <c r="O44" s="28" t="str">
         <f>CONCATENATE("M 1 ",'Elimination Matches'!G7)</f>
       </c>
     </row>
     <row r="46">
       <c r="F46" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G46" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="G46" s="23"/>
       <c r="N46" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="O46" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="O46" s="23"/>
     </row>
     <row r="47">
       <c r="F47" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G47" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="G47" s="23"/>
       <c r="N47" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="O47" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="O47" s="23"/>
     </row>
     <row r="50">
-      <c r="A50" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="I50" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="20"/>
-      <c r="M50" s="20"/>
-      <c r="N50" s="20"/>
-      <c r="O50" s="20"/>
+      <c r="A50" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="24"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
+      <c r="I50" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="J50" s="24"/>
+      <c r="K50" s="24"/>
+      <c r="L50" s="24"/>
+      <c r="M50" s="24"/>
+      <c r="N50" s="24"/>
+      <c r="O50" s="24"/>
     </row>
     <row r="51">
-      <c r="A51" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D51" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G51" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="I51" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="L51" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="O51" s="35" t="s">
-        <v>78</v>
+      <c r="A51" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G51" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="I51" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="L51" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="O51" s="39" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="24" t="str">
+      <c r="A52" s="28" t="str">
         <f>'data'!B7</f>
       </c>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24" t="str">
+      <c r="B52" s="28"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="28" t="str">
         <f>CONCATENATE("M 2 ",'Elimination Matches'!O7)</f>
       </c>
-      <c r="I52" s="24" t="str">
+      <c r="I52" s="28" t="str">
         <f>'data'!B10</f>
       </c>
-      <c r="J52" s="24"/>
-      <c r="K52" s="24"/>
-      <c r="L52" s="24"/>
-      <c r="M52" s="24"/>
-      <c r="N52" s="24"/>
-      <c r="O52" s="24" t="str">
+      <c r="J52" s="28"/>
+      <c r="K52" s="28"/>
+      <c r="L52" s="28"/>
+      <c r="M52" s="28"/>
+      <c r="N52" s="28"/>
+      <c r="O52" s="28" t="str">
         <f>CONCATENATE("M 3 ",'Elimination Matches'!G15)</f>
       </c>
     </row>
     <row r="54">
       <c r="F54" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G54" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="G54" s="23"/>
       <c r="N54" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="O54" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="O54" s="23"/>
     </row>
     <row r="55">
       <c r="F55" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G55" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="G55" s="23"/>
       <c r="N55" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="O55" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="O55" s="23"/>
     </row>
     <row r="58">
-      <c r="A58" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="20"/>
-      <c r="I58" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="J58" s="20"/>
-      <c r="K58" s="20"/>
-      <c r="L58" s="20"/>
-      <c r="M58" s="20"/>
-      <c r="N58" s="20"/>
-      <c r="O58" s="20"/>
+      <c r="A58" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B58" s="24"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="I58" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="J58" s="24"/>
+      <c r="K58" s="24"/>
+      <c r="L58" s="24"/>
+      <c r="M58" s="24"/>
+      <c r="N58" s="24"/>
+      <c r="O58" s="24"/>
     </row>
     <row r="59">
-      <c r="A59" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D59" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G59" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="I59" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="L59" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="O59" s="37" t="s">
-        <v>78</v>
+      <c r="A59" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D59" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G59" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="I59" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="L59" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="O59" s="41" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="24" t="str">
+      <c r="A60" s="28" t="str">
         <f>'data'!B13</f>
       </c>
-      <c r="B60" s="24"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
-      <c r="G60" s="24" t="str">
+      <c r="B60" s="28"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="28"/>
+      <c r="F60" s="28"/>
+      <c r="G60" s="28" t="str">
         <f>CONCATENATE("M 4 ",'Elimination Matches'!O15)</f>
       </c>
-      <c r="I60" s="24" t="str">
+      <c r="I60" s="28" t="str">
         <f>'data'!B16</f>
       </c>
-      <c r="J60" s="24"/>
-      <c r="K60" s="24"/>
-      <c r="L60" s="24"/>
-      <c r="M60" s="24"/>
-      <c r="N60" s="24"/>
-      <c r="O60" s="24" t="str">
+      <c r="J60" s="28"/>
+      <c r="K60" s="28"/>
+      <c r="L60" s="28"/>
+      <c r="M60" s="28"/>
+      <c r="N60" s="28"/>
+      <c r="O60" s="28" t="str">
         <f>CONCATENATE("M 5 ",'Elimination Matches'!G23)</f>
       </c>
     </row>
     <row r="62">
       <c r="F62" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G62" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="G62" s="23"/>
       <c r="N62" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="O62" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="O62" s="23"/>
     </row>
     <row r="63">
       <c r="F63" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G63" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="G63" s="23"/>
       <c r="N63" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="O63" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="O63" s="23"/>
     </row>
     <row r="66">
-      <c r="A66" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B66" s="20"/>
-      <c r="C66" s="20"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="20"/>
-      <c r="G66" s="20"/>
-      <c r="I66" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="J66" s="20"/>
-      <c r="K66" s="20"/>
-      <c r="L66" s="20"/>
-      <c r="M66" s="20"/>
-      <c r="N66" s="20"/>
-      <c r="O66" s="20"/>
+      <c r="A66" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B66" s="24"/>
+      <c r="C66" s="24"/>
+      <c r="D66" s="24"/>
+      <c r="E66" s="24"/>
+      <c r="F66" s="24"/>
+      <c r="G66" s="24"/>
+      <c r="I66" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="J66" s="24"/>
+      <c r="K66" s="24"/>
+      <c r="L66" s="24"/>
+      <c r="M66" s="24"/>
+      <c r="N66" s="24"/>
+      <c r="O66" s="24"/>
     </row>
     <row r="67">
-      <c r="A67" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D67" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G67" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="I67" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="L67" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="O67" s="39" t="s">
-        <v>78</v>
+      <c r="A67" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D67" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G67" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="I67" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="L67" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="O67" s="43" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="24" t="str">
+      <c r="A68" s="28" t="str">
         <f>'data'!B19</f>
       </c>
-      <c r="B68" s="24"/>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="24"/>
-      <c r="F68" s="24"/>
-      <c r="G68" s="24" t="str">
+      <c r="B68" s="28"/>
+      <c r="C68" s="28"/>
+      <c r="D68" s="28"/>
+      <c r="E68" s="28"/>
+      <c r="F68" s="28"/>
+      <c r="G68" s="28" t="str">
         <f>CONCATENATE("M 6 ",'Elimination Matches'!O23)</f>
       </c>
-      <c r="I68" s="24" t="str">
+      <c r="I68" s="28" t="str">
         <f>'data'!B22</f>
       </c>
-      <c r="J68" s="24"/>
-      <c r="K68" s="24"/>
-      <c r="L68" s="24"/>
-      <c r="M68" s="24"/>
-      <c r="N68" s="24"/>
-      <c r="O68" s="24" t="str">
+      <c r="J68" s="28"/>
+      <c r="K68" s="28"/>
+      <c r="L68" s="28"/>
+      <c r="M68" s="28"/>
+      <c r="N68" s="28"/>
+      <c r="O68" s="28" t="str">
         <f>CONCATENATE("M 7 ",'Elimination Matches'!G31)</f>
       </c>
     </row>
     <row r="70">
       <c r="F70" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G70" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="G70" s="23"/>
       <c r="N70" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="O70" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="O70" s="23"/>
     </row>
     <row r="71">
       <c r="F71" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G71" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="G71" s="23"/>
       <c r="N71" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="O71" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="O71" s="23"/>
     </row>
     <row r="79">
-      <c r="A79" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B79" s="20"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="20"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="20"/>
-      <c r="G79" s="20"/>
-      <c r="H79" s="20"/>
-      <c r="I79" s="20"/>
-      <c r="J79" s="20"/>
-      <c r="K79" s="20"/>
-      <c r="L79" s="20"/>
-      <c r="M79" s="20"/>
-      <c r="N79" s="20"/>
-      <c r="O79" s="20"/>
+      <c r="A79" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B79" s="24"/>
+      <c r="C79" s="24"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="24"/>
+      <c r="H79" s="24"/>
+      <c r="I79" s="24"/>
+      <c r="J79" s="24"/>
+      <c r="K79" s="24"/>
+      <c r="L79" s="24"/>
+      <c r="M79" s="24"/>
+      <c r="N79" s="24"/>
+      <c r="O79" s="24"/>
     </row>
     <row r="81">
-      <c r="A81" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="B81" s="20"/>
-      <c r="C81" s="20"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="20"/>
-      <c r="F81" s="20"/>
-      <c r="G81" s="20"/>
-      <c r="I81" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="J81" s="20"/>
-      <c r="K81" s="20"/>
-      <c r="L81" s="20"/>
-      <c r="M81" s="20"/>
-      <c r="N81" s="20"/>
-      <c r="O81" s="20"/>
+      <c r="A81" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B81" s="24"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="24"/>
+      <c r="I81" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="J81" s="24"/>
+      <c r="K81" s="24"/>
+      <c r="L81" s="24"/>
+      <c r="M81" s="24"/>
+      <c r="N81" s="24"/>
+      <c r="O81" s="24"/>
     </row>
     <row r="82">
-      <c r="A82" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D82" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G82" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="I82" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="L82" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="O82" s="41" t="s">
-        <v>78</v>
+      <c r="A82" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D82" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G82" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="I82" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="L82" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="O82" s="45" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="24" t="str">
+      <c r="A83" s="28" t="str">
         <f>CONCATENATE("M 8 ",'Elimination Matches'!G46)</f>
       </c>
-      <c r="B83" s="24"/>
-      <c r="C83" s="24"/>
-      <c r="D83" s="24"/>
-      <c r="E83" s="24"/>
-      <c r="F83" s="24"/>
-      <c r="G83" s="24" t="str">
+      <c r="B83" s="28"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="28"/>
+      <c r="F83" s="28"/>
+      <c r="G83" s="28" t="str">
         <f>CONCATENATE("M 9 ",'Elimination Matches'!O46)</f>
       </c>
-      <c r="I83" s="24" t="str">
+      <c r="I83" s="28" t="str">
         <f>CONCATENATE("M 10 ",'Elimination Matches'!G54)</f>
       </c>
-      <c r="J83" s="24"/>
-      <c r="K83" s="24"/>
-      <c r="L83" s="24"/>
-      <c r="M83" s="24"/>
-      <c r="N83" s="24"/>
-      <c r="O83" s="24" t="str">
+      <c r="J83" s="28"/>
+      <c r="K83" s="28"/>
+      <c r="L83" s="28"/>
+      <c r="M83" s="28"/>
+      <c r="N83" s="28"/>
+      <c r="O83" s="28" t="str">
         <f>CONCATENATE("M 11 ",'Elimination Matches'!O54)</f>
       </c>
     </row>
     <row r="85">
       <c r="F85" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G85" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="G85" s="23"/>
       <c r="N85" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="O85" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="O85" s="23"/>
     </row>
     <row r="86">
       <c r="F86" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G86" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="G86" s="23"/>
       <c r="N86" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="O86" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="O86" s="23"/>
     </row>
     <row r="89">
-      <c r="A89" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B89" s="20"/>
-      <c r="C89" s="20"/>
-      <c r="D89" s="20"/>
-      <c r="E89" s="20"/>
-      <c r="F89" s="20"/>
-      <c r="G89" s="20"/>
-      <c r="I89" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="J89" s="20"/>
-      <c r="K89" s="20"/>
-      <c r="L89" s="20"/>
-      <c r="M89" s="20"/>
-      <c r="N89" s="20"/>
-      <c r="O89" s="20"/>
+      <c r="A89" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B89" s="24"/>
+      <c r="C89" s="24"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="24"/>
+      <c r="I89" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="J89" s="24"/>
+      <c r="K89" s="24"/>
+      <c r="L89" s="24"/>
+      <c r="M89" s="24"/>
+      <c r="N89" s="24"/>
+      <c r="O89" s="24"/>
     </row>
     <row r="90">
-      <c r="A90" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D90" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G90" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="I90" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="L90" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="O90" s="43" t="s">
-        <v>78</v>
+      <c r="A90" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D90" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G90" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="I90" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="L90" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="O90" s="47" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="24" t="str">
+      <c r="A91" s="28" t="str">
         <f>CONCATENATE("M 12 ",'Elimination Matches'!G62)</f>
       </c>
-      <c r="B91" s="24"/>
-      <c r="C91" s="24"/>
-      <c r="D91" s="24"/>
-      <c r="E91" s="24"/>
-      <c r="F91" s="24"/>
-      <c r="G91" s="24" t="str">
+      <c r="B91" s="28"/>
+      <c r="C91" s="28"/>
+      <c r="D91" s="28"/>
+      <c r="E91" s="28"/>
+      <c r="F91" s="28"/>
+      <c r="G91" s="28" t="str">
         <f>CONCATENATE("M 13 ",'Elimination Matches'!O62)</f>
       </c>
-      <c r="I91" s="24" t="str">
+      <c r="I91" s="28" t="str">
         <f>CONCATENATE("M 14 ",'Elimination Matches'!G70)</f>
       </c>
-      <c r="J91" s="24"/>
-      <c r="K91" s="24"/>
-      <c r="L91" s="24"/>
-      <c r="M91" s="24"/>
-      <c r="N91" s="24"/>
-      <c r="O91" s="24" t="str">
+      <c r="J91" s="28"/>
+      <c r="K91" s="28"/>
+      <c r="L91" s="28"/>
+      <c r="M91" s="28"/>
+      <c r="N91" s="28"/>
+      <c r="O91" s="28" t="str">
         <f>CONCATENATE("M 15 ",'Elimination Matches'!O70)</f>
       </c>
     </row>
     <row r="93">
       <c r="F93" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G93" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="G93" s="23"/>
       <c r="N93" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="O93" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="O93" s="23"/>
     </row>
     <row r="94">
       <c r="F94" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G94" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="G94" s="23"/>
       <c r="N94" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="O94" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="O94" s="23"/>
     </row>
     <row r="102">
-      <c r="A102" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B102" s="20"/>
-      <c r="C102" s="20"/>
-      <c r="D102" s="20"/>
-      <c r="E102" s="20"/>
-      <c r="F102" s="20"/>
-      <c r="G102" s="20"/>
-      <c r="H102" s="20"/>
-      <c r="I102" s="20"/>
-      <c r="J102" s="20"/>
-      <c r="K102" s="20"/>
-      <c r="L102" s="20"/>
-      <c r="M102" s="20"/>
-      <c r="N102" s="20"/>
-      <c r="O102" s="20"/>
+      <c r="A102" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="B102" s="24"/>
+      <c r="C102" s="24"/>
+      <c r="D102" s="24"/>
+      <c r="E102" s="24"/>
+      <c r="F102" s="24"/>
+      <c r="G102" s="24"/>
+      <c r="H102" s="24"/>
+      <c r="I102" s="24"/>
+      <c r="J102" s="24"/>
+      <c r="K102" s="24"/>
+      <c r="L102" s="24"/>
+      <c r="M102" s="24"/>
+      <c r="N102" s="24"/>
+      <c r="O102" s="24"/>
     </row>
     <row r="104">
-      <c r="A104" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="B104" s="20"/>
-      <c r="C104" s="20"/>
-      <c r="D104" s="20"/>
-      <c r="E104" s="20"/>
-      <c r="F104" s="20"/>
-      <c r="G104" s="20"/>
-      <c r="I104" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="J104" s="20"/>
-      <c r="K104" s="20"/>
-      <c r="L104" s="20"/>
-      <c r="M104" s="20"/>
-      <c r="N104" s="20"/>
-      <c r="O104" s="20"/>
+      <c r="A104" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B104" s="24"/>
+      <c r="C104" s="24"/>
+      <c r="D104" s="24"/>
+      <c r="E104" s="24"/>
+      <c r="F104" s="24"/>
+      <c r="G104" s="24"/>
+      <c r="I104" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="J104" s="24"/>
+      <c r="K104" s="24"/>
+      <c r="L104" s="24"/>
+      <c r="M104" s="24"/>
+      <c r="N104" s="24"/>
+      <c r="O104" s="24"/>
     </row>
     <row r="105">
-      <c r="A105" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D105" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G105" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="I105" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="L105" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="O105" s="45" t="s">
-        <v>78</v>
+      <c r="A105" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D105" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G105" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="I105" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="L105" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="O105" s="49" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="24" t="str">
+      <c r="A106" s="28" t="str">
         <f>CONCATENATE("M 16 ",'Elimination Matches'!G85)</f>
       </c>
-      <c r="B106" s="24"/>
-      <c r="C106" s="24"/>
-      <c r="D106" s="24"/>
-      <c r="E106" s="24"/>
-      <c r="F106" s="24"/>
-      <c r="G106" s="24" t="str">
+      <c r="B106" s="28"/>
+      <c r="C106" s="28"/>
+      <c r="D106" s="28"/>
+      <c r="E106" s="28"/>
+      <c r="F106" s="28"/>
+      <c r="G106" s="28" t="str">
         <f>CONCATENATE("M 17 ",'Elimination Matches'!O85)</f>
       </c>
-      <c r="I106" s="24" t="str">
+      <c r="I106" s="28" t="str">
         <f>CONCATENATE("M 18 ",'Elimination Matches'!G93)</f>
       </c>
-      <c r="J106" s="24"/>
-      <c r="K106" s="24"/>
-      <c r="L106" s="24"/>
-      <c r="M106" s="24"/>
-      <c r="N106" s="24"/>
-      <c r="O106" s="24" t="str">
+      <c r="J106" s="28"/>
+      <c r="K106" s="28"/>
+      <c r="L106" s="28"/>
+      <c r="M106" s="28"/>
+      <c r="N106" s="28"/>
+      <c r="O106" s="28" t="str">
         <f>CONCATENATE("M 19 ",'Elimination Matches'!O93)</f>
       </c>
     </row>
     <row r="108">
       <c r="F108" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G108" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="G108" s="23"/>
       <c r="N108" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="O108" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="O108" s="23"/>
     </row>
     <row r="109">
       <c r="F109" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G109" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="G109" s="23"/>
       <c r="N109" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="O109" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="O109" s="23"/>
     </row>
     <row r="117">
-      <c r="A117" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="B117" s="20"/>
-      <c r="C117" s="20"/>
-      <c r="D117" s="20"/>
-      <c r="E117" s="20"/>
-      <c r="F117" s="20"/>
-      <c r="G117" s="20"/>
-      <c r="H117" s="20"/>
-      <c r="I117" s="20"/>
-      <c r="J117" s="20"/>
-      <c r="K117" s="20"/>
-      <c r="L117" s="20"/>
-      <c r="M117" s="20"/>
-      <c r="N117" s="20"/>
-      <c r="O117" s="20"/>
+      <c r="A117" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B117" s="24"/>
+      <c r="C117" s="24"/>
+      <c r="D117" s="24"/>
+      <c r="E117" s="24"/>
+      <c r="F117" s="24"/>
+      <c r="G117" s="24"/>
+      <c r="H117" s="24"/>
+      <c r="I117" s="24"/>
+      <c r="J117" s="24"/>
+      <c r="K117" s="24"/>
+      <c r="L117" s="24"/>
+      <c r="M117" s="24"/>
+      <c r="N117" s="24"/>
+      <c r="O117" s="24"/>
     </row>
     <row r="119">
-      <c r="A119" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="B119" s="20"/>
-      <c r="C119" s="20"/>
-      <c r="D119" s="20"/>
-      <c r="E119" s="20"/>
-      <c r="F119" s="20"/>
-      <c r="G119" s="20"/>
+      <c r="A119" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B119" s="24"/>
+      <c r="C119" s="24"/>
+      <c r="D119" s="24"/>
+      <c r="E119" s="24"/>
+      <c r="F119" s="24"/>
+      <c r="G119" s="24"/>
     </row>
     <row r="120">
-      <c r="A120" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D120" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G120" s="46" t="s">
-        <v>78</v>
+      <c r="A120" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D120" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G120" s="50" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="24" t="str">
+      <c r="A121" s="28" t="str">
         <f>CONCATENATE("M 20 ",'Elimination Matches'!G108)</f>
       </c>
-      <c r="B121" s="24"/>
-      <c r="C121" s="24"/>
-      <c r="D121" s="24"/>
-      <c r="E121" s="24"/>
-      <c r="F121" s="24"/>
-      <c r="G121" s="24" t="str">
+      <c r="B121" s="28"/>
+      <c r="C121" s="28"/>
+      <c r="D121" s="28"/>
+      <c r="E121" s="28"/>
+      <c r="F121" s="28"/>
+      <c r="G121" s="28" t="str">
         <f>CONCATENATE("M 21 ",'Elimination Matches'!O108)</f>
       </c>
     </row>
     <row r="123">
       <c r="F123" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G123" s="19"/>
+        <v>88</v>
+      </c>
+      <c r="G123" s="23"/>
     </row>
     <row r="124">
       <c r="F124" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G124" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="G124" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="27">
@@ -3769,7 +4355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA952CF-7580-BA4A-BFF2-63054D7F5497}">
   <sheetPr>
     <pageSetUpPr fitToPage="true"/>
@@ -3788,280 +4374,280 @@
   </cols>
   <sheetData>
     <row r="1" ht="110" customHeight="true">
-      <c r="A1" s="21">
+      <c r="A1" s="25">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="str">
+      <c r="B1" s="26" t="str">
         <f>data!D2</f>
       </c>
     </row>
     <row r="2" ht="115" customHeight="true">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" ht="110" customHeight="true">
-      <c r="A3" s="21">
+      <c r="A3" s="25">
         <v>1</v>
       </c>
-      <c r="B3" s="22" t="str">
+      <c r="B3" s="26" t="str">
         <f>data!D3</f>
       </c>
     </row>
     <row r="4" ht="115" customHeight="true">
-      <c r="A4" s="21"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="26"/>
     </row>
     <row r="5" ht="110" customHeight="true">
-      <c r="A5" s="21">
+      <c r="A5" s="25">
         <v>2</v>
       </c>
-      <c r="B5" s="22" t="str">
+      <c r="B5" s="26" t="str">
         <f>data!D4</f>
       </c>
     </row>
     <row r="6" ht="115" customHeight="true">
-      <c r="A6" s="21"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="26"/>
     </row>
     <row r="7" ht="110" customHeight="true">
-      <c r="A7" s="21">
+      <c r="A7" s="25">
         <v>3</v>
       </c>
-      <c r="B7" s="22" t="str">
+      <c r="B7" s="26" t="str">
         <f>data!D5</f>
       </c>
     </row>
     <row r="8" ht="115" customHeight="true">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="26"/>
     </row>
     <row r="9" ht="110" customHeight="true">
-      <c r="A9" s="21">
+      <c r="A9" s="25">
         <v>4</v>
       </c>
-      <c r="B9" s="22" t="str">
+      <c r="B9" s="26" t="str">
         <f>data!D6</f>
       </c>
     </row>
     <row r="10" ht="115" customHeight="true">
-      <c r="A10" s="21"/>
-      <c r="B10" s="22"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
     </row>
     <row r="11" ht="110" customHeight="true">
-      <c r="A11" s="21">
+      <c r="A11" s="25">
         <v>5</v>
       </c>
-      <c r="B11" s="22" t="str">
+      <c r="B11" s="26" t="str">
         <f>data!D7</f>
       </c>
     </row>
     <row r="12" ht="115" customHeight="true">
-      <c r="A12" s="21"/>
-      <c r="B12" s="22"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="26"/>
     </row>
     <row r="13" ht="110" customHeight="true">
-      <c r="A13" s="21">
+      <c r="A13" s="25">
         <v>6</v>
       </c>
-      <c r="B13" s="22" t="str">
+      <c r="B13" s="26" t="str">
         <f>data!D8</f>
       </c>
     </row>
     <row r="14" ht="115" customHeight="true">
-      <c r="A14" s="21"/>
-      <c r="B14" s="22"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="26"/>
     </row>
     <row r="15" ht="110" customHeight="true">
-      <c r="A15" s="21">
+      <c r="A15" s="25">
         <v>7</v>
       </c>
-      <c r="B15" s="22" t="str">
+      <c r="B15" s="26" t="str">
         <f>data!D9</f>
       </c>
     </row>
     <row r="16" ht="115" customHeight="true">
-      <c r="A16" s="21"/>
-      <c r="B16" s="22"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
     </row>
     <row r="17" ht="110" customHeight="true">
-      <c r="A17" s="21">
+      <c r="A17" s="25">
         <v>8</v>
       </c>
-      <c r="B17" s="22" t="str">
+      <c r="B17" s="26" t="str">
         <f>data!D10</f>
       </c>
     </row>
     <row r="18" ht="115" customHeight="true">
-      <c r="A18" s="21"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
     </row>
     <row r="19" ht="110" customHeight="true">
-      <c r="A19" s="21">
+      <c r="A19" s="25">
         <v>9</v>
       </c>
-      <c r="B19" s="22" t="str">
+      <c r="B19" s="26" t="str">
         <f>data!D11</f>
       </c>
     </row>
     <row r="20" ht="115" customHeight="true">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
     </row>
     <row r="21" ht="110" customHeight="true">
-      <c r="A21" s="21">
+      <c r="A21" s="25">
         <v>10</v>
       </c>
-      <c r="B21" s="22" t="str">
+      <c r="B21" s="26" t="str">
         <f>data!D12</f>
       </c>
     </row>
     <row r="22" ht="115" customHeight="true">
-      <c r="A22" s="21"/>
-      <c r="B22" s="22"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
     </row>
     <row r="23" ht="110" customHeight="true">
-      <c r="A23" s="21">
+      <c r="A23" s="25">
         <v>11</v>
       </c>
-      <c r="B23" s="22" t="str">
+      <c r="B23" s="26" t="str">
         <f>data!D13</f>
       </c>
     </row>
     <row r="24" ht="115" customHeight="true">
-      <c r="A24" s="21"/>
-      <c r="B24" s="22"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="26"/>
     </row>
     <row r="25" ht="110" customHeight="true">
-      <c r="A25" s="21">
+      <c r="A25" s="25">
         <v>12</v>
       </c>
-      <c r="B25" s="22" t="str">
+      <c r="B25" s="26" t="str">
         <f>data!D14</f>
       </c>
     </row>
     <row r="26" ht="115" customHeight="true">
-      <c r="A26" s="21"/>
-      <c r="B26" s="22"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
     </row>
     <row r="27" ht="110" customHeight="true">
-      <c r="A27" s="21">
+      <c r="A27" s="25">
         <v>13</v>
       </c>
-      <c r="B27" s="22" t="str">
+      <c r="B27" s="26" t="str">
         <f>data!D15</f>
       </c>
     </row>
     <row r="28" ht="115" customHeight="true">
-      <c r="A28" s="21"/>
-      <c r="B28" s="22"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="26"/>
     </row>
     <row r="29" ht="110" customHeight="true">
-      <c r="A29" s="21">
+      <c r="A29" s="25">
         <v>14</v>
       </c>
-      <c r="B29" s="22" t="str">
+      <c r="B29" s="26" t="str">
         <f>data!D16</f>
       </c>
     </row>
     <row r="30" ht="115" customHeight="true">
-      <c r="A30" s="21"/>
-      <c r="B30" s="22"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="26"/>
     </row>
     <row r="31" ht="110" customHeight="true">
-      <c r="A31" s="21">
+      <c r="A31" s="25">
         <v>15</v>
       </c>
-      <c r="B31" s="22" t="str">
+      <c r="B31" s="26" t="str">
         <f>data!D17</f>
       </c>
     </row>
     <row r="32" ht="115" customHeight="true">
-      <c r="A32" s="21"/>
-      <c r="B32" s="22"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="26"/>
     </row>
     <row r="33" ht="110" customHeight="true">
-      <c r="A33" s="21">
+      <c r="A33" s="25">
         <v>16</v>
       </c>
-      <c r="B33" s="22" t="str">
+      <c r="B33" s="26" t="str">
         <f>data!D18</f>
       </c>
     </row>
     <row r="34" ht="115" customHeight="true">
-      <c r="A34" s="21"/>
-      <c r="B34" s="22"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="26"/>
     </row>
     <row r="35" ht="110" customHeight="true">
-      <c r="A35" s="21">
+      <c r="A35" s="25">
         <v>17</v>
       </c>
-      <c r="B35" s="22" t="str">
+      <c r="B35" s="26" t="str">
         <f>data!D19</f>
       </c>
     </row>
     <row r="36" ht="115" customHeight="true">
-      <c r="A36" s="21"/>
-      <c r="B36" s="22"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="26"/>
     </row>
     <row r="37" ht="110" customHeight="true">
-      <c r="A37" s="21">
+      <c r="A37" s="25">
         <v>18</v>
       </c>
-      <c r="B37" s="22" t="str">
+      <c r="B37" s="26" t="str">
         <f>data!D20</f>
       </c>
     </row>
     <row r="38" ht="115" customHeight="true">
-      <c r="A38" s="21"/>
-      <c r="B38" s="22"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="26"/>
     </row>
     <row r="39" ht="110" customHeight="true">
-      <c r="A39" s="21">
+      <c r="A39" s="25">
         <v>19</v>
       </c>
-      <c r="B39" s="22" t="str">
+      <c r="B39" s="26" t="str">
         <f>data!D21</f>
       </c>
     </row>
     <row r="40" ht="115" customHeight="true">
-      <c r="A40" s="21"/>
-      <c r="B40" s="22"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="26"/>
     </row>
     <row r="41" ht="110" customHeight="true">
-      <c r="A41" s="21">
+      <c r="A41" s="25">
         <v>20</v>
       </c>
-      <c r="B41" s="22" t="str">
+      <c r="B41" s="26" t="str">
         <f>data!D22</f>
       </c>
     </row>
     <row r="42" ht="115" customHeight="true">
-      <c r="A42" s="21"/>
-      <c r="B42" s="22"/>
+      <c r="A42" s="25"/>
+      <c r="B42" s="26"/>
     </row>
     <row r="43" ht="110" customHeight="true">
-      <c r="A43" s="21">
+      <c r="A43" s="25">
         <v>21</v>
       </c>
-      <c r="B43" s="22" t="str">
+      <c r="B43" s="26" t="str">
         <f>data!D23</f>
       </c>
     </row>
     <row r="44" ht="115" customHeight="true">
-      <c r="A44" s="21"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="26"/>
     </row>
     <row r="45" ht="110" customHeight="true">
-      <c r="A45" s="21">
+      <c r="A45" s="25">
         <v>22</v>
       </c>
-      <c r="B45" s="22" t="str">
+      <c r="B45" s="26" t="str">
         <f>data!D24</f>
       </c>
     </row>
     <row r="46" ht="115" customHeight="true">
-      <c r="A46" s="21"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="23">
@@ -4093,335 +4679,4 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" horizontalDpi="0" orientation="landscape" paperSize="8" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4065E12-1BC4-BF48-9DCD-AFB9407081DC}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="true"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showGridLines="false" view="pageLayout" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P56" sqref="P56"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="13"/>
-  <cols>
-    <col customWidth="true" max="1" min="1" width="20.83203125"/>
-    <col customWidth="true" max="3" min="3" width="20"/>
-    <col customWidth="true" max="5" min="5" width="20"/>
-  </cols>
-  <sheetData>
-    <row r="6">
-      <c r="E6" s="20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="E7" s="20"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="8">
-      <c r="G8" s="16"/>
-    </row>
-    <row r="9">
-      <c r="G9" s="16"/>
-    </row>
-    <row r="10">
-      <c r="G10" s="17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="G11" s="16"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="16"/>
-    </row>
-    <row r="12">
-      <c r="G12" s="16"/>
-      <c r="I12" s="16"/>
-    </row>
-    <row r="13">
-      <c r="E13" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="16"/>
-      <c r="I13" s="16"/>
-    </row>
-    <row r="14">
-      <c r="E14" s="20"/>
-      <c r="I14" s="16"/>
-    </row>
-    <row r="15">
-      <c r="I15" s="16"/>
-    </row>
-    <row r="16">
-      <c r="I16" s="16"/>
-    </row>
-    <row r="17">
-      <c r="I17" s="16"/>
-    </row>
-    <row r="18">
-      <c r="I18" s="17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="I19" s="16"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="16"/>
-    </row>
-    <row r="20">
-      <c r="I20" s="16"/>
-      <c r="K20" s="16"/>
-    </row>
-    <row r="21">
-      <c r="E21" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="16"/>
-      <c r="K21" s="16"/>
-    </row>
-    <row r="22">
-      <c r="E22" s="20"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="K22" s="16"/>
-    </row>
-    <row r="23">
-      <c r="G23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="K23" s="16"/>
-    </row>
-    <row r="24">
-      <c r="G24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="K24" s="16"/>
-    </row>
-    <row r="25">
-      <c r="G25" s="17">
-        <v>9</v>
-      </c>
-      <c r="H25" s="19"/>
-      <c r="I25" s="16"/>
-      <c r="K25" s="16"/>
-    </row>
-    <row r="26">
-      <c r="C26" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="16"/>
-      <c r="K26" s="16"/>
-    </row>
-    <row r="27">
-      <c r="C27" s="20"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="K27" s="16"/>
-    </row>
-    <row r="28">
-      <c r="E28" s="17">
-        <v>1</v>
-      </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="16"/>
-      <c r="K28" s="16"/>
-    </row>
-    <row r="29">
-      <c r="C29" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="16"/>
-      <c r="K29" s="16"/>
-    </row>
-    <row r="30">
-      <c r="C30" s="20"/>
-      <c r="K30" s="16"/>
-    </row>
-    <row r="31">
-      <c r="K31" s="16"/>
-    </row>
-    <row r="32">
-      <c r="K32" s="16"/>
-    </row>
-    <row r="33">
-      <c r="K33" s="16"/>
-    </row>
-    <row r="34">
-      <c r="K34" s="17">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="K35" s="16"/>
-    </row>
-    <row r="36">
-      <c r="K36" s="16"/>
-    </row>
-    <row r="37">
-      <c r="E37" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="K37" s="16"/>
-    </row>
-    <row r="38">
-      <c r="E38" s="20"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="16"/>
-      <c r="K38" s="16"/>
-    </row>
-    <row r="39">
-      <c r="G39" s="16"/>
-      <c r="K39" s="16"/>
-    </row>
-    <row r="40">
-      <c r="G40" s="16"/>
-      <c r="K40" s="16"/>
-    </row>
-    <row r="41">
-      <c r="G41" s="17">
-        <v>10</v>
-      </c>
-      <c r="K41" s="16"/>
-    </row>
-    <row r="42">
-      <c r="C42" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="G42" s="16"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="16"/>
-      <c r="K42" s="16"/>
-    </row>
-    <row r="43">
-      <c r="C43" s="20"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="I43" s="16"/>
-      <c r="K43" s="16"/>
-    </row>
-    <row r="44">
-      <c r="E44" s="17">
-        <v>2</v>
-      </c>
-      <c r="F44" s="19"/>
-      <c r="G44" s="16"/>
-      <c r="I44" s="16"/>
-      <c r="K44" s="16"/>
-    </row>
-    <row r="45">
-      <c r="C45" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="16"/>
-      <c r="I45" s="16"/>
-      <c r="K45" s="16"/>
-    </row>
-    <row r="46">
-      <c r="C46" s="20"/>
-      <c r="I46" s="16"/>
-      <c r="K46" s="16"/>
-    </row>
-    <row r="47">
-      <c r="I47" s="16"/>
-      <c r="K47" s="16"/>
-    </row>
-    <row r="48">
-      <c r="I48" s="16"/>
-      <c r="K48" s="16"/>
-    </row>
-    <row r="49">
-      <c r="I49" s="17">
-        <v>17</v>
-      </c>
-      <c r="J49" s="19"/>
-      <c r="K49" s="16"/>
-    </row>
-    <row r="50">
-      <c r="I50" s="16"/>
-    </row>
-    <row r="51">
-      <c r="I51" s="16"/>
-    </row>
-    <row r="52">
-      <c r="E52" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="I52" s="16"/>
-    </row>
-    <row r="53">
-      <c r="E53" s="20"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="16"/>
-      <c r="I53" s="16"/>
-    </row>
-    <row r="54">
-      <c r="G54" s="16"/>
-      <c r="I54" s="16"/>
-    </row>
-    <row r="55">
-      <c r="G55" s="16"/>
-      <c r="I55" s="16"/>
-    </row>
-    <row r="56">
-      <c r="G56" s="17">
-        <v>11</v>
-      </c>
-      <c r="H56" s="19"/>
-      <c r="I56" s="16"/>
-    </row>
-    <row r="57">
-      <c r="C57" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="G57" s="16"/>
-    </row>
-    <row r="58">
-      <c r="C58" s="20"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="16"/>
-      <c r="G58" s="16"/>
-    </row>
-    <row r="59">
-      <c r="E59" s="17">
-        <v>3</v>
-      </c>
-      <c r="F59" s="19"/>
-      <c r="G59" s="16"/>
-    </row>
-    <row r="60">
-      <c r="C60" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D60" s="19"/>
-      <c r="E60" s="16"/>
-    </row>
-    <row r="61">
-      <c r="C61" s="20"/>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C60:C61"/>
-  </mergeCells>
-  <printOptions horizontalCentered="true" verticalCentered="true"/>
-  <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
make examples deterministic and update them with the new tree
</commit_message>
<xml_diff>
--- a/playoffs-example-medium.xlsx
+++ b/playoffs-example-medium.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="21580" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="26060" windowHeight="21580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -88,6 +88,204 @@
     <t>Display Name</t>
   </si>
   <si>
+    <t>Cersei Lannister</t>
+  </si>
+  <si>
+    <t>Team Gamma</t>
+  </si>
+  <si>
+    <t>C. LANNISTER</t>
+  </si>
+  <si>
+    <t>Daenerys Targaryen</t>
+  </si>
+  <si>
+    <t>Team Delta</t>
+  </si>
+  <si>
+    <t>D. TARGARYEN</t>
+  </si>
+  <si>
+    <t>Eddard Stark</t>
+  </si>
+  <si>
+    <t>Team Epsilon</t>
+  </si>
+  <si>
+    <t>E. STARK</t>
+  </si>
+  <si>
+    <t>Frodo Baggins</t>
+  </si>
+  <si>
+    <t>Team Zeta</t>
+  </si>
+  <si>
+    <t>F. BAGGINS</t>
+  </si>
+  <si>
+    <t>Gandalf The Grey</t>
+  </si>
+  <si>
+    <t>Team Eta</t>
+  </si>
+  <si>
+    <t>G. GREY</t>
+  </si>
+  <si>
+    <t>Hermione Granger</t>
+  </si>
+  <si>
+    <t>Team Theta</t>
+  </si>
+  <si>
+    <t>H. GRANGER</t>
+  </si>
+  <si>
+    <t>Inigo Montoya</t>
+  </si>
+  <si>
+    <t>Team Iota</t>
+  </si>
+  <si>
+    <t>I. MONTOYA</t>
+  </si>
+  <si>
+    <t>Jon Snow</t>
+  </si>
+  <si>
+    <t>Team Kappa</t>
+  </si>
+  <si>
+    <t>J. SNOW</t>
+  </si>
+  <si>
+    <t>Katniss Everdeen</t>
+  </si>
+  <si>
+    <t>Team Lambda</t>
+  </si>
+  <si>
+    <t>K. EVERDEEN</t>
+  </si>
+  <si>
+    <t>Legolas Greenleaf</t>
+  </si>
+  <si>
+    <t>Team Mu</t>
+  </si>
+  <si>
+    <t>L. GREENLEAF</t>
+  </si>
+  <si>
+    <t>Moby Dick</t>
+  </si>
+  <si>
+    <t>Team Nu</t>
+  </si>
+  <si>
+    <t>M. DICK</t>
+  </si>
+  <si>
+    <t>Neville Longbottom</t>
+  </si>
+  <si>
+    <t>Team Xi</t>
+  </si>
+  <si>
+    <t>N. LONGBOTTOM</t>
+  </si>
+  <si>
+    <t>Othello</t>
+  </si>
+  <si>
+    <t>Team Omicron</t>
+  </si>
+  <si>
+    <t>O. OTHELLO</t>
+  </si>
+  <si>
+    <t>Petyr Baelish</t>
+  </si>
+  <si>
+    <t>Team Pi</t>
+  </si>
+  <si>
+    <t>P. BAELISH</t>
+  </si>
+  <si>
+    <t>Quirinus Quirrell</t>
+  </si>
+  <si>
+    <t>Team Rho</t>
+  </si>
+  <si>
+    <t>Q. QUIRRELL</t>
+  </si>
+  <si>
+    <t>Ron Weasley</t>
+  </si>
+  <si>
+    <t>Team Sigma</t>
+  </si>
+  <si>
+    <t>R. WEASLEY</t>
+  </si>
+  <si>
+    <t>Samwise Gamgee</t>
+  </si>
+  <si>
+    <t>Team Tau</t>
+  </si>
+  <si>
+    <t>S. GAMGEE</t>
+  </si>
+  <si>
+    <t>Tyrion Lannister</t>
+  </si>
+  <si>
+    <t>Team Upsilon</t>
+  </si>
+  <si>
+    <t>T. LANNISTER</t>
+  </si>
+  <si>
+    <t>Ulysses</t>
+  </si>
+  <si>
+    <t>Team Phi</t>
+  </si>
+  <si>
+    <t>U. ULYSSES</t>
+  </si>
+  <si>
+    <t>Voldemort</t>
+  </si>
+  <si>
+    <t>Team Chi</t>
+  </si>
+  <si>
+    <t>V. VOLDEMORT</t>
+  </si>
+  <si>
+    <t>Willy Wonka</t>
+  </si>
+  <si>
+    <t>Team Psi</t>
+  </si>
+  <si>
+    <t>W. WONKA</t>
+  </si>
+  <si>
+    <t>Xaro Xhoan Daxos</t>
+  </si>
+  <si>
+    <t>Team Omega</t>
+  </si>
+  <si>
+    <t>X. DAXOS</t>
+  </si>
+  <si>
     <t>Ygritte</t>
   </si>
   <si>
@@ -95,204 +293,6 @@
   </si>
   <si>
     <t>Y. YGRITTE</t>
-  </si>
-  <si>
-    <t>Tyrion Lannister</t>
-  </si>
-  <si>
-    <t>Team Upsilon</t>
-  </si>
-  <si>
-    <t>T. LANNISTER</t>
-  </si>
-  <si>
-    <t>Xaro Xhoan Daxos</t>
-  </si>
-  <si>
-    <t>Team Omega</t>
-  </si>
-  <si>
-    <t>X. DAXOS</t>
-  </si>
-  <si>
-    <t>Ulysses</t>
-  </si>
-  <si>
-    <t>Team Phi</t>
-  </si>
-  <si>
-    <t>U. ULYSSES</t>
-  </si>
-  <si>
-    <t>Jon Snow</t>
-  </si>
-  <si>
-    <t>Team Kappa</t>
-  </si>
-  <si>
-    <t>J. SNOW</t>
-  </si>
-  <si>
-    <t>Frodo Baggins</t>
-  </si>
-  <si>
-    <t>Team Zeta</t>
-  </si>
-  <si>
-    <t>F. BAGGINS</t>
-  </si>
-  <si>
-    <t>Eddard Stark</t>
-  </si>
-  <si>
-    <t>Team Epsilon</t>
-  </si>
-  <si>
-    <t>E. STARK</t>
-  </si>
-  <si>
-    <t>Othello</t>
-  </si>
-  <si>
-    <t>Team Omicron</t>
-  </si>
-  <si>
-    <t>O. OTHELLO</t>
-  </si>
-  <si>
-    <t>Daenerys Targaryen</t>
-  </si>
-  <si>
-    <t>Team Delta</t>
-  </si>
-  <si>
-    <t>D. TARGARYEN</t>
-  </si>
-  <si>
-    <t>Cersei Lannister</t>
-  </si>
-  <si>
-    <t>Team Gamma</t>
-  </si>
-  <si>
-    <t>C. LANNISTER</t>
-  </si>
-  <si>
-    <t>Ron Weasley</t>
-  </si>
-  <si>
-    <t>Team Sigma</t>
-  </si>
-  <si>
-    <t>R. WEASLEY</t>
-  </si>
-  <si>
-    <t>Inigo Montoya</t>
-  </si>
-  <si>
-    <t>Team Iota</t>
-  </si>
-  <si>
-    <t>I. MONTOYA</t>
-  </si>
-  <si>
-    <t>Quirinus Quirrell</t>
-  </si>
-  <si>
-    <t>Team Rho</t>
-  </si>
-  <si>
-    <t>Q. QUIRRELL</t>
-  </si>
-  <si>
-    <t>Willy Wonka</t>
-  </si>
-  <si>
-    <t>Team Psi</t>
-  </si>
-  <si>
-    <t>W. WONKA</t>
-  </si>
-  <si>
-    <t>Moby Dick</t>
-  </si>
-  <si>
-    <t>Team Nu</t>
-  </si>
-  <si>
-    <t>M. DICK</t>
-  </si>
-  <si>
-    <t>Katniss Everdeen</t>
-  </si>
-  <si>
-    <t>Team Lambda</t>
-  </si>
-  <si>
-    <t>K. EVERDEEN</t>
-  </si>
-  <si>
-    <t>Samwise Gamgee</t>
-  </si>
-  <si>
-    <t>Team Tau</t>
-  </si>
-  <si>
-    <t>S. GAMGEE</t>
-  </si>
-  <si>
-    <t>Neville Longbottom</t>
-  </si>
-  <si>
-    <t>Team Xi</t>
-  </si>
-  <si>
-    <t>N. LONGBOTTOM</t>
-  </si>
-  <si>
-    <t>Legolas Greenleaf</t>
-  </si>
-  <si>
-    <t>Team Mu</t>
-  </si>
-  <si>
-    <t>L. GREENLEAF</t>
-  </si>
-  <si>
-    <t>Petyr Baelish</t>
-  </si>
-  <si>
-    <t>Team Pi</t>
-  </si>
-  <si>
-    <t>P. BAELISH</t>
-  </si>
-  <si>
-    <t>Gandalf The Grey</t>
-  </si>
-  <si>
-    <t>Team Eta</t>
-  </si>
-  <si>
-    <t>G. GREY</t>
-  </si>
-  <si>
-    <t>Voldemort</t>
-  </si>
-  <si>
-    <t>Team Chi</t>
-  </si>
-  <si>
-    <t>V. VOLDEMORT</t>
-  </si>
-  <si>
-    <t>Hermione Granger</t>
-  </si>
-  <si>
-    <t>Team Theta</t>
-  </si>
-  <si>
-    <t>H. GRANGER</t>
   </si>
   <si>
     <t>Match 1</t>
@@ -645,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -704,13 +704,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
@@ -2389,325 +2392,204 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="false" view="pageLayout" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P56" sqref="P56"/>
+    <sheetView showGridLines="false" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.5" defaultRowHeight="13"/>
   <cols>
     <col customWidth="true" max="1" min="1" width="20.83203125"/>
-    <col customWidth="true" max="3" min="3" width="20"/>
-    <col customWidth="true" max="5" min="5" width="20"/>
+    <col customWidth="true" max="2" min="2" width="10"/>
   </cols>
   <sheetData>
+    <row r="2">
+      <c r="E2" s="24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="F3" s="22"/>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4">
+      <c r="G4" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="G5" s="20"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="20"/>
+    </row>
     <row r="6">
       <c r="E6" s="24" t="s">
-        <v>17</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F6" s="23"/>
+      <c r="G6" s="20"/>
+      <c r="I6" s="20"/>
     </row>
     <row r="7">
-      <c r="E7" s="24"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="20"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="8">
-      <c r="G8" s="20"/>
+      <c r="I8" s="21">
+        <v>16</v>
+      </c>
     </row>
     <row r="9">
-      <c r="G9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="20"/>
     </row>
     <row r="10">
-      <c r="G10" s="21">
-        <v>8</v>
-      </c>
+      <c r="E10" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="20"/>
+      <c r="K10" s="20"/>
     </row>
     <row r="11">
+      <c r="F11" s="22"/>
       <c r="G11" s="20"/>
-      <c r="H11" s="22"/>
       <c r="I11" s="20"/>
+      <c r="K11" s="20"/>
     </row>
     <row r="12">
-      <c r="G12" s="20"/>
+      <c r="G12" s="21">
+        <v>9</v>
+      </c>
+      <c r="H12" s="23"/>
       <c r="I12" s="20"/>
+      <c r="K12" s="20"/>
     </row>
     <row r="13">
-      <c r="E13" s="24" t="s">
+      <c r="C13" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="20"/>
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14">
+      <c r="D14" s="22"/>
+      <c r="E14" s="21">
+        <v>1</v>
+      </c>
+      <c r="F14" s="23"/>
+      <c r="G14" s="20"/>
+      <c r="K14" s="20"/>
+    </row>
+    <row r="15">
+      <c r="C15" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="23"/>
+      <c r="E15" s="20"/>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16">
+      <c r="K16" s="21">
         <v>20</v>
       </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="20"/>
-      <c r="I13" s="20"/>
-    </row>
-    <row r="14">
-      <c r="E14" s="24"/>
-      <c r="I14" s="20"/>
-    </row>
-    <row r="15">
-      <c r="I15" s="20"/>
-    </row>
-    <row r="16">
-      <c r="I16" s="20"/>
     </row>
     <row r="17">
-      <c r="I17" s="20"/>
+      <c r="K17" s="20"/>
     </row>
     <row r="18">
-      <c r="I18" s="21">
-        <v>16</v>
-      </c>
+      <c r="E18" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="K18" s="20"/>
     </row>
     <row r="19">
-      <c r="I19" s="20"/>
-      <c r="J19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="20"/>
       <c r="K19" s="20"/>
     </row>
     <row r="20">
-      <c r="I20" s="20"/>
+      <c r="G20" s="21">
+        <v>10</v>
+      </c>
       <c r="K20" s="20"/>
     </row>
     <row r="21">
-      <c r="E21" s="24" t="s">
-        <v>23</v>
-      </c>
+      <c r="C21" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="20"/>
+      <c r="H21" s="22"/>
       <c r="I21" s="20"/>
       <c r="K21" s="20"/>
     </row>
     <row r="22">
-      <c r="E22" s="24"/>
-      <c r="F22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="21">
+        <v>2</v>
+      </c>
+      <c r="F22" s="23"/>
       <c r="G22" s="20"/>
       <c r="I22" s="20"/>
       <c r="K22" s="20"/>
     </row>
     <row r="23">
-      <c r="G23" s="20"/>
+      <c r="C23" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="23"/>
+      <c r="E23" s="20"/>
       <c r="I23" s="20"/>
       <c r="K23" s="20"/>
     </row>
     <row r="24">
-      <c r="G24" s="20"/>
-      <c r="I24" s="20"/>
+      <c r="I24" s="21">
+        <v>17</v>
+      </c>
+      <c r="J24" s="23"/>
       <c r="K24" s="20"/>
     </row>
     <row r="25">
-      <c r="G25" s="21">
-        <v>9</v>
-      </c>
-      <c r="H25" s="23"/>
       <c r="I25" s="20"/>
-      <c r="K25" s="20"/>
     </row>
     <row r="26">
-      <c r="C26" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="G26" s="20"/>
-      <c r="K26" s="20"/>
+      <c r="E26" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26" s="20"/>
     </row>
     <row r="27">
-      <c r="C27" s="24"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="20"/>
+      <c r="F27" s="22"/>
       <c r="G27" s="20"/>
-      <c r="K27" s="20"/>
+      <c r="I27" s="20"/>
     </row>
     <row r="28">
-      <c r="E28" s="21">
-        <v>1</v>
-      </c>
-      <c r="F28" s="23"/>
-      <c r="G28" s="20"/>
-      <c r="K28" s="20"/>
+      <c r="G28" s="21">
+        <v>11</v>
+      </c>
+      <c r="H28" s="23"/>
+      <c r="I28" s="20"/>
     </row>
     <row r="29">
       <c r="C29" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="20"/>
-      <c r="K29" s="20"/>
+        <v>44</v>
+      </c>
+      <c r="G29" s="20"/>
     </row>
     <row r="30">
-      <c r="C30" s="24"/>
-      <c r="K30" s="20"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="21">
+        <v>3</v>
+      </c>
+      <c r="F30" s="23"/>
+      <c r="G30" s="20"/>
     </row>
     <row r="31">
-      <c r="K31" s="20"/>
-    </row>
-    <row r="32">
-      <c r="K32" s="20"/>
-    </row>
-    <row r="33">
-      <c r="K33" s="20"/>
-    </row>
-    <row r="34">
-      <c r="K34" s="21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="K35" s="20"/>
-    </row>
-    <row r="36">
-      <c r="K36" s="20"/>
-    </row>
-    <row r="37">
-      <c r="E37" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="K37" s="20"/>
-    </row>
-    <row r="38">
-      <c r="E38" s="24"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="20"/>
-      <c r="K38" s="20"/>
-    </row>
-    <row r="39">
-      <c r="G39" s="20"/>
-      <c r="K39" s="20"/>
-    </row>
-    <row r="40">
-      <c r="G40" s="20"/>
-      <c r="K40" s="20"/>
-    </row>
-    <row r="41">
-      <c r="G41" s="21">
-        <v>10</v>
-      </c>
-      <c r="K41" s="20"/>
-    </row>
-    <row r="42">
-      <c r="C42" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="G42" s="20"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="20"/>
-      <c r="K42" s="20"/>
-    </row>
-    <row r="43">
-      <c r="C43" s="24"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="K43" s="20"/>
-    </row>
-    <row r="44">
-      <c r="E44" s="21">
-        <v>2</v>
-      </c>
-      <c r="F44" s="23"/>
-      <c r="G44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="K44" s="20"/>
-    </row>
-    <row r="45">
-      <c r="C45" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D45" s="23"/>
-      <c r="E45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="K45" s="20"/>
-    </row>
-    <row r="46">
-      <c r="C46" s="24"/>
-      <c r="I46" s="20"/>
-      <c r="K46" s="20"/>
-    </row>
-    <row r="47">
-      <c r="I47" s="20"/>
-      <c r="K47" s="20"/>
-    </row>
-    <row r="48">
-      <c r="I48" s="20"/>
-      <c r="K48" s="20"/>
-    </row>
-    <row r="49">
-      <c r="I49" s="21">
-        <v>17</v>
-      </c>
-      <c r="J49" s="23"/>
-      <c r="K49" s="20"/>
-    </row>
-    <row r="50">
-      <c r="I50" s="20"/>
-    </row>
-    <row r="51">
-      <c r="I51" s="20"/>
-    </row>
-    <row r="52">
-      <c r="E52" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="I52" s="20"/>
-    </row>
-    <row r="53">
-      <c r="E53" s="24"/>
-      <c r="F53" s="22"/>
-      <c r="G53" s="20"/>
-      <c r="I53" s="20"/>
-    </row>
-    <row r="54">
-      <c r="G54" s="20"/>
-      <c r="I54" s="20"/>
-    </row>
-    <row r="55">
-      <c r="G55" s="20"/>
-      <c r="I55" s="20"/>
-    </row>
-    <row r="56">
-      <c r="G56" s="21">
-        <v>11</v>
-      </c>
-      <c r="H56" s="23"/>
-      <c r="I56" s="20"/>
-    </row>
-    <row r="57">
-      <c r="C57" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="G57" s="20"/>
-    </row>
-    <row r="58">
-      <c r="C58" s="24"/>
-      <c r="D58" s="22"/>
-      <c r="E58" s="20"/>
-      <c r="G58" s="20"/>
-    </row>
-    <row r="59">
-      <c r="E59" s="21">
-        <v>3</v>
-      </c>
-      <c r="F59" s="23"/>
-      <c r="G59" s="20"/>
-    </row>
-    <row r="60">
-      <c r="C60" s="24" t="s">
+      <c r="C31" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="D60" s="23"/>
-      <c r="E60" s="20"/>
-    </row>
-    <row r="61">
-      <c r="C61" s="24"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C60:C61"/>
-  </mergeCells>
   <printOptions horizontalCentered="true" verticalCentered="true"/>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2720,337 +2602,213 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="false" view="pageLayout" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P56" sqref="P56"/>
+    <sheetView showGridLines="false" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.5" defaultRowHeight="13"/>
   <cols>
     <col customWidth="true" max="1" min="1" width="20.83203125"/>
-    <col customWidth="true" max="3" min="3" width="20"/>
-    <col customWidth="true" max="5" min="5" width="20"/>
+    <col customWidth="true" max="2" min="2" width="10"/>
   </cols>
   <sheetData>
+    <row r="2">
+      <c r="E2" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="F3" s="22"/>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4">
+      <c r="G4" s="21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="20"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="20"/>
+    </row>
     <row r="6">
-      <c r="E6" s="24" t="s">
-        <v>50</v>
-      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="21">
+        <v>4</v>
+      </c>
+      <c r="F6" s="23"/>
+      <c r="G6" s="20"/>
+      <c r="I6" s="20"/>
     </row>
     <row r="7">
-      <c r="E7" s="24"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="20"/>
+      <c r="C7" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="20"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="8">
-      <c r="G8" s="20"/>
+      <c r="I8" s="21">
+        <v>18</v>
+      </c>
     </row>
     <row r="9">
-      <c r="G9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="20"/>
     </row>
     <row r="10">
-      <c r="G10" s="21">
-        <v>12</v>
-      </c>
+      <c r="E10" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="20"/>
+      <c r="K10" s="20"/>
     </row>
     <row r="11">
-      <c r="C11" s="24" t="s">
-        <v>53</v>
-      </c>
+      <c r="F11" s="22"/>
       <c r="G11" s="20"/>
-      <c r="H11" s="22"/>
       <c r="I11" s="20"/>
+      <c r="K11" s="20"/>
     </row>
     <row r="12">
-      <c r="C12" s="24"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="20"/>
-      <c r="G12" s="20"/>
+      <c r="G12" s="21">
+        <v>13</v>
+      </c>
+      <c r="H12" s="23"/>
       <c r="I12" s="20"/>
+      <c r="K12" s="20"/>
     </row>
     <row r="13">
-      <c r="E13" s="21">
-        <v>4</v>
-      </c>
-      <c r="F13" s="23"/>
+      <c r="C13" s="24" t="s">
+        <v>62</v>
+      </c>
       <c r="G13" s="20"/>
-      <c r="I13" s="20"/>
+      <c r="K13" s="20"/>
     </row>
     <row r="14">
-      <c r="C14" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="20"/>
-      <c r="I14" s="20"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="21">
+        <v>5</v>
+      </c>
+      <c r="F14" s="23"/>
+      <c r="G14" s="20"/>
+      <c r="K14" s="20"/>
     </row>
     <row r="15">
-      <c r="C15" s="24"/>
-      <c r="I15" s="20"/>
+      <c r="C15" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="23"/>
+      <c r="E15" s="20"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16">
-      <c r="I16" s="20"/>
+      <c r="K16" s="21">
+        <v>21</v>
+      </c>
     </row>
     <row r="17">
-      <c r="I17" s="20"/>
+      <c r="K17" s="20"/>
     </row>
     <row r="18">
-      <c r="I18" s="21">
-        <v>18</v>
-      </c>
+      <c r="E18" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="K18" s="20"/>
     </row>
     <row r="19">
-      <c r="I19" s="20"/>
-      <c r="J19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="20"/>
       <c r="K19" s="20"/>
     </row>
     <row r="20">
-      <c r="I20" s="20"/>
+      <c r="G20" s="21">
+        <v>14</v>
+      </c>
       <c r="K20" s="20"/>
     </row>
     <row r="21">
-      <c r="E21" s="24" t="s">
-        <v>59</v>
-      </c>
+      <c r="C21" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="20"/>
+      <c r="H21" s="22"/>
       <c r="I21" s="20"/>
       <c r="K21" s="20"/>
     </row>
     <row r="22">
-      <c r="E22" s="24"/>
-      <c r="F22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="21">
+        <v>6</v>
+      </c>
+      <c r="F22" s="23"/>
       <c r="G22" s="20"/>
       <c r="I22" s="20"/>
       <c r="K22" s="20"/>
     </row>
     <row r="23">
-      <c r="G23" s="20"/>
+      <c r="C23" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="23"/>
+      <c r="E23" s="20"/>
       <c r="I23" s="20"/>
       <c r="K23" s="20"/>
     </row>
     <row r="24">
-      <c r="G24" s="20"/>
-      <c r="I24" s="20"/>
+      <c r="I24" s="21">
+        <v>19</v>
+      </c>
+      <c r="J24" s="23"/>
       <c r="K24" s="20"/>
     </row>
     <row r="25">
-      <c r="G25" s="21">
-        <v>13</v>
-      </c>
-      <c r="H25" s="23"/>
       <c r="I25" s="20"/>
-      <c r="K25" s="20"/>
     </row>
     <row r="26">
-      <c r="C26" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="G26" s="20"/>
-      <c r="K26" s="20"/>
+      <c r="E26" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="I26" s="20"/>
     </row>
     <row r="27">
-      <c r="C27" s="24"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="20"/>
+      <c r="F27" s="22"/>
       <c r="G27" s="20"/>
-      <c r="K27" s="20"/>
+      <c r="I27" s="20"/>
     </row>
     <row r="28">
-      <c r="E28" s="21">
-        <v>5</v>
-      </c>
-      <c r="F28" s="23"/>
-      <c r="G28" s="20"/>
-      <c r="K28" s="20"/>
+      <c r="G28" s="21">
+        <v>15</v>
+      </c>
+      <c r="H28" s="23"/>
+      <c r="I28" s="20"/>
     </row>
     <row r="29">
       <c r="C29" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="20"/>
-      <c r="K29" s="20"/>
+        <v>80</v>
+      </c>
+      <c r="G29" s="20"/>
     </row>
     <row r="30">
-      <c r="C30" s="24"/>
-      <c r="K30" s="20"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="21">
+        <v>7</v>
+      </c>
+      <c r="F30" s="23"/>
+      <c r="G30" s="20"/>
     </row>
     <row r="31">
-      <c r="K31" s="20"/>
-    </row>
-    <row r="32">
-      <c r="K32" s="20"/>
-    </row>
-    <row r="33">
-      <c r="K33" s="20"/>
-    </row>
-    <row r="34">
-      <c r="K34" s="21">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="K35" s="20"/>
-    </row>
-    <row r="36">
-      <c r="K36" s="20"/>
-    </row>
-    <row r="37">
-      <c r="E37" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="K37" s="20"/>
-    </row>
-    <row r="38">
-      <c r="E38" s="24"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="20"/>
-      <c r="K38" s="20"/>
-    </row>
-    <row r="39">
-      <c r="G39" s="20"/>
-      <c r="K39" s="20"/>
-    </row>
-    <row r="40">
-      <c r="G40" s="20"/>
-      <c r="K40" s="20"/>
-    </row>
-    <row r="41">
-      <c r="G41" s="21">
-        <v>14</v>
-      </c>
-      <c r="K41" s="20"/>
-    </row>
-    <row r="42">
-      <c r="C42" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="G42" s="20"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="20"/>
-      <c r="K42" s="20"/>
-    </row>
-    <row r="43">
-      <c r="C43" s="24"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="K43" s="20"/>
-    </row>
-    <row r="44">
-      <c r="E44" s="21">
-        <v>6</v>
-      </c>
-      <c r="F44" s="23"/>
-      <c r="G44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="K44" s="20"/>
-    </row>
-    <row r="45">
-      <c r="C45" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="D45" s="23"/>
-      <c r="E45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="K45" s="20"/>
-    </row>
-    <row r="46">
-      <c r="C46" s="24"/>
-      <c r="I46" s="20"/>
-      <c r="K46" s="20"/>
-    </row>
-    <row r="47">
-      <c r="I47" s="20"/>
-      <c r="K47" s="20"/>
-    </row>
-    <row r="48">
-      <c r="I48" s="20"/>
-      <c r="K48" s="20"/>
-    </row>
-    <row r="49">
-      <c r="I49" s="21">
-        <v>19</v>
-      </c>
-      <c r="J49" s="23"/>
-      <c r="K49" s="20"/>
-    </row>
-    <row r="50">
-      <c r="I50" s="20"/>
-    </row>
-    <row r="51">
-      <c r="I51" s="20"/>
-    </row>
-    <row r="52">
-      <c r="E52" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="I52" s="20"/>
-    </row>
-    <row r="53">
-      <c r="E53" s="24"/>
-      <c r="F53" s="22"/>
-      <c r="G53" s="20"/>
-      <c r="I53" s="20"/>
-    </row>
-    <row r="54">
-      <c r="G54" s="20"/>
-      <c r="I54" s="20"/>
-    </row>
-    <row r="55">
-      <c r="G55" s="20"/>
-      <c r="I55" s="20"/>
-    </row>
-    <row r="56">
-      <c r="G56" s="21">
-        <v>15</v>
-      </c>
-      <c r="H56" s="23"/>
-      <c r="I56" s="20"/>
-    </row>
-    <row r="57">
-      <c r="C57" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="G57" s="20"/>
-    </row>
-    <row r="58">
-      <c r="C58" s="24"/>
-      <c r="D58" s="22"/>
-      <c r="E58" s="20"/>
-      <c r="G58" s="20"/>
-    </row>
-    <row r="59">
-      <c r="E59" s="21">
-        <v>7</v>
-      </c>
-      <c r="F59" s="23"/>
-      <c r="G59" s="20"/>
-    </row>
-    <row r="60">
-      <c r="C60" s="24" t="s">
+      <c r="C31" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D60" s="23"/>
-      <c r="E60" s="20"/>
-    </row>
-    <row r="61">
-      <c r="C61" s="24"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C60:C61"/>
-  </mergeCells>
   <printOptions horizontalCentered="true" verticalCentered="true"/>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3103,7 +2861,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="11">
         <v>0</v>
@@ -3213,7 +2971,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="12">
         <v>2.7777777777777779E-3</v>
@@ -3293,85 +3051,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="true">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
     </row>
     <row r="3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="I3" s="24" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="I3" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
     </row>
     <row r="4">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="L4" s="28" t="s">
+      <c r="L4" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="O4" s="30" t="s">
+      <c r="O4" s="31" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="28" t="str">
+      <c r="A5" s="29" t="str">
         <f>'data'!B5</f>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28" t="str">
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29" t="str">
         <f>'data'!B6</f>
       </c>
-      <c r="I5" s="28" t="str">
+      <c r="I5" s="29" t="str">
         <f>'data'!B8</f>
       </c>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28" t="str">
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29" t="str">
         <f>'data'!B9</f>
       </c>
     </row>
@@ -3396,66 +3154,66 @@
       <c r="O8" s="23"/>
     </row>
     <row r="11">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="I11" s="24" t="s">
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="I11" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
     </row>
     <row r="12">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="I12" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="L12" s="28" t="s">
+      <c r="L12" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="O12" s="32" t="s">
+      <c r="O12" s="33" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="28" t="str">
+      <c r="A13" s="29" t="str">
         <f>'data'!B11</f>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28" t="str">
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29" t="str">
         <f>'data'!B12</f>
       </c>
-      <c r="I13" s="28" t="str">
+      <c r="I13" s="29" t="str">
         <f>'data'!B14</f>
       </c>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28" t="str">
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29" t="str">
         <f>'data'!B15</f>
       </c>
     </row>
@@ -3480,66 +3238,66 @@
       <c r="O16" s="23"/>
     </row>
     <row r="19">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="I19" s="24" t="s">
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="I19" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
+      <c r="O19" s="27"/>
     </row>
     <row r="20">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="G20" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="I20" s="27" t="s">
+      <c r="I20" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="L20" s="28" t="s">
+      <c r="L20" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="O20" s="34" t="s">
+      <c r="O20" s="35" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="28" t="str">
+      <c r="A21" s="29" t="str">
         <f>'data'!B17</f>
       </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28" t="str">
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29" t="str">
         <f>'data'!B18</f>
       </c>
-      <c r="I21" s="28" t="str">
+      <c r="I21" s="29" t="str">
         <f>'data'!B20</f>
       </c>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="28" t="str">
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29" t="str">
         <f>'data'!B21</f>
       </c>
     </row>
@@ -3564,37 +3322,37 @@
       <c r="O24" s="23"/>
     </row>
     <row r="27">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
     </row>
     <row r="28">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="G28" s="35" t="s">
+      <c r="G28" s="36" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="28" t="str">
+      <c r="A29" s="29" t="str">
         <f>'data'!B23</f>
       </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28" t="str">
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29" t="str">
         <f>'data'!B24</f>
       </c>
     </row>
@@ -3611,85 +3369,85 @@
       <c r="G32" s="23"/>
     </row>
     <row r="40">
-      <c r="A40" s="24" t="s">
+      <c r="A40" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="24"/>
-      <c r="L40" s="24"/>
-      <c r="M40" s="24"/>
-      <c r="N40" s="24"/>
-      <c r="O40" s="24"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
+      <c r="N40" s="27"/>
+      <c r="O40" s="27"/>
     </row>
     <row r="42">
-      <c r="A42" s="24" t="s">
+      <c r="A42" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
-      <c r="I42" s="24" t="s">
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="I42" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="J42" s="24"/>
-      <c r="K42" s="24"/>
-      <c r="L42" s="24"/>
-      <c r="M42" s="24"/>
-      <c r="N42" s="24"/>
-      <c r="O42" s="24"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="27"/>
+      <c r="M42" s="27"/>
+      <c r="N42" s="27"/>
+      <c r="O42" s="27"/>
     </row>
     <row r="43">
-      <c r="A43" s="27" t="s">
+      <c r="A43" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="G43" s="36" t="s">
+      <c r="G43" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="I43" s="27" t="s">
+      <c r="I43" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="L43" s="28" t="s">
+      <c r="L43" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="O43" s="37" t="s">
+      <c r="O43" s="38" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="28" t="str">
+      <c r="A44" s="29" t="str">
         <f>'data'!B2</f>
       </c>
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="28" t="str">
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29" t="str">
         <f>'data'!B3</f>
       </c>
-      <c r="I44" s="28" t="str">
+      <c r="I44" s="29" t="str">
         <f>'data'!B4</f>
       </c>
-      <c r="J44" s="28"/>
-      <c r="K44" s="28"/>
-      <c r="L44" s="28"/>
-      <c r="M44" s="28"/>
-      <c r="N44" s="28"/>
-      <c r="O44" s="28" t="str">
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="29"/>
+      <c r="N44" s="29"/>
+      <c r="O44" s="29" t="str">
         <f>CONCATENATE("M 1 ",'Elimination Matches'!G7)</f>
       </c>
     </row>
@@ -3714,66 +3472,66 @@
       <c r="O47" s="23"/>
     </row>
     <row r="50">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="24"/>
-      <c r="I50" s="24" t="s">
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="27"/>
+      <c r="I50" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J50" s="24"/>
-      <c r="K50" s="24"/>
-      <c r="L50" s="24"/>
-      <c r="M50" s="24"/>
-      <c r="N50" s="24"/>
-      <c r="O50" s="24"/>
+      <c r="J50" s="27"/>
+      <c r="K50" s="27"/>
+      <c r="L50" s="27"/>
+      <c r="M50" s="27"/>
+      <c r="N50" s="27"/>
+      <c r="O50" s="27"/>
     </row>
     <row r="51">
-      <c r="A51" s="27" t="s">
+      <c r="A51" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="28" t="s">
+      <c r="D51" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="G51" s="38" t="s">
+      <c r="G51" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="I51" s="27" t="s">
+      <c r="I51" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="L51" s="28" t="s">
+      <c r="L51" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="O51" s="39" t="s">
+      <c r="O51" s="40" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="28" t="str">
+      <c r="A52" s="29" t="str">
         <f>'data'!B7</f>
       </c>
-      <c r="B52" s="28"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="28"/>
-      <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="28" t="str">
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29" t="str">
         <f>CONCATENATE("M 2 ",'Elimination Matches'!O7)</f>
       </c>
-      <c r="I52" s="28" t="str">
+      <c r="I52" s="29" t="str">
         <f>'data'!B10</f>
       </c>
-      <c r="J52" s="28"/>
-      <c r="K52" s="28"/>
-      <c r="L52" s="28"/>
-      <c r="M52" s="28"/>
-      <c r="N52" s="28"/>
-      <c r="O52" s="28" t="str">
+      <c r="J52" s="29"/>
+      <c r="K52" s="29"/>
+      <c r="L52" s="29"/>
+      <c r="M52" s="29"/>
+      <c r="N52" s="29"/>
+      <c r="O52" s="29" t="str">
         <f>CONCATENATE("M 3 ",'Elimination Matches'!G15)</f>
       </c>
     </row>
@@ -3798,66 +3556,66 @@
       <c r="O55" s="23"/>
     </row>
     <row r="58">
-      <c r="A58" s="24" t="s">
+      <c r="A58" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="B58" s="24"/>
-      <c r="C58" s="24"/>
-      <c r="D58" s="24"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="24"/>
-      <c r="I58" s="24" t="s">
+      <c r="B58" s="27"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
+      <c r="F58" s="27"/>
+      <c r="G58" s="27"/>
+      <c r="I58" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="J58" s="24"/>
-      <c r="K58" s="24"/>
-      <c r="L58" s="24"/>
-      <c r="M58" s="24"/>
-      <c r="N58" s="24"/>
-      <c r="O58" s="24"/>
+      <c r="J58" s="27"/>
+      <c r="K58" s="27"/>
+      <c r="L58" s="27"/>
+      <c r="M58" s="27"/>
+      <c r="N58" s="27"/>
+      <c r="O58" s="27"/>
     </row>
     <row r="59">
-      <c r="A59" s="27" t="s">
+      <c r="A59" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D59" s="28" t="s">
+      <c r="D59" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="G59" s="40" t="s">
+      <c r="G59" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="I59" s="27" t="s">
+      <c r="I59" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="L59" s="28" t="s">
+      <c r="L59" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="O59" s="41" t="s">
+      <c r="O59" s="42" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="28" t="str">
+      <c r="A60" s="29" t="str">
         <f>'data'!B13</f>
       </c>
-      <c r="B60" s="28"/>
-      <c r="C60" s="28"/>
-      <c r="D60" s="28"/>
-      <c r="E60" s="28"/>
-      <c r="F60" s="28"/>
-      <c r="G60" s="28" t="str">
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="29"/>
+      <c r="G60" s="29" t="str">
         <f>CONCATENATE("M 4 ",'Elimination Matches'!O15)</f>
       </c>
-      <c r="I60" s="28" t="str">
+      <c r="I60" s="29" t="str">
         <f>'data'!B16</f>
       </c>
-      <c r="J60" s="28"/>
-      <c r="K60" s="28"/>
-      <c r="L60" s="28"/>
-      <c r="M60" s="28"/>
-      <c r="N60" s="28"/>
-      <c r="O60" s="28" t="str">
+      <c r="J60" s="29"/>
+      <c r="K60" s="29"/>
+      <c r="L60" s="29"/>
+      <c r="M60" s="29"/>
+      <c r="N60" s="29"/>
+      <c r="O60" s="29" t="str">
         <f>CONCATENATE("M 5 ",'Elimination Matches'!G23)</f>
       </c>
     </row>
@@ -3882,66 +3640,66 @@
       <c r="O63" s="23"/>
     </row>
     <row r="66">
-      <c r="A66" s="24" t="s">
+      <c r="A66" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="B66" s="24"/>
-      <c r="C66" s="24"/>
-      <c r="D66" s="24"/>
-      <c r="E66" s="24"/>
-      <c r="F66" s="24"/>
-      <c r="G66" s="24"/>
-      <c r="I66" s="24" t="s">
+      <c r="B66" s="27"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="27"/>
+      <c r="F66" s="27"/>
+      <c r="G66" s="27"/>
+      <c r="I66" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="J66" s="24"/>
-      <c r="K66" s="24"/>
-      <c r="L66" s="24"/>
-      <c r="M66" s="24"/>
-      <c r="N66" s="24"/>
-      <c r="O66" s="24"/>
+      <c r="J66" s="27"/>
+      <c r="K66" s="27"/>
+      <c r="L66" s="27"/>
+      <c r="M66" s="27"/>
+      <c r="N66" s="27"/>
+      <c r="O66" s="27"/>
     </row>
     <row r="67">
-      <c r="A67" s="27" t="s">
+      <c r="A67" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D67" s="28" t="s">
+      <c r="D67" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="G67" s="42" t="s">
+      <c r="G67" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="I67" s="27" t="s">
+      <c r="I67" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="L67" s="28" t="s">
+      <c r="L67" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="O67" s="43" t="s">
+      <c r="O67" s="44" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="28" t="str">
+      <c r="A68" s="29" t="str">
         <f>'data'!B19</f>
       </c>
-      <c r="B68" s="28"/>
-      <c r="C68" s="28"/>
-      <c r="D68" s="28"/>
-      <c r="E68" s="28"/>
-      <c r="F68" s="28"/>
-      <c r="G68" s="28" t="str">
+      <c r="B68" s="29"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="29"/>
+      <c r="F68" s="29"/>
+      <c r="G68" s="29" t="str">
         <f>CONCATENATE("M 6 ",'Elimination Matches'!O23)</f>
       </c>
-      <c r="I68" s="28" t="str">
+      <c r="I68" s="29" t="str">
         <f>'data'!B22</f>
       </c>
-      <c r="J68" s="28"/>
-      <c r="K68" s="28"/>
-      <c r="L68" s="28"/>
-      <c r="M68" s="28"/>
-      <c r="N68" s="28"/>
-      <c r="O68" s="28" t="str">
+      <c r="J68" s="29"/>
+      <c r="K68" s="29"/>
+      <c r="L68" s="29"/>
+      <c r="M68" s="29"/>
+      <c r="N68" s="29"/>
+      <c r="O68" s="29" t="str">
         <f>CONCATENATE("M 7 ",'Elimination Matches'!G31)</f>
       </c>
     </row>
@@ -3966,85 +3724,85 @@
       <c r="O71" s="23"/>
     </row>
     <row r="79">
-      <c r="A79" s="24" t="s">
+      <c r="A79" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="B79" s="24"/>
-      <c r="C79" s="24"/>
-      <c r="D79" s="24"/>
-      <c r="E79" s="24"/>
-      <c r="F79" s="24"/>
-      <c r="G79" s="24"/>
-      <c r="H79" s="24"/>
-      <c r="I79" s="24"/>
-      <c r="J79" s="24"/>
-      <c r="K79" s="24"/>
-      <c r="L79" s="24"/>
-      <c r="M79" s="24"/>
-      <c r="N79" s="24"/>
-      <c r="O79" s="24"/>
+      <c r="B79" s="27"/>
+      <c r="C79" s="27"/>
+      <c r="D79" s="27"/>
+      <c r="E79" s="27"/>
+      <c r="F79" s="27"/>
+      <c r="G79" s="27"/>
+      <c r="H79" s="27"/>
+      <c r="I79" s="27"/>
+      <c r="J79" s="27"/>
+      <c r="K79" s="27"/>
+      <c r="L79" s="27"/>
+      <c r="M79" s="27"/>
+      <c r="N79" s="27"/>
+      <c r="O79" s="27"/>
     </row>
     <row r="81">
-      <c r="A81" s="24" t="s">
+      <c r="A81" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="B81" s="24"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
-      <c r="E81" s="24"/>
-      <c r="F81" s="24"/>
-      <c r="G81" s="24"/>
-      <c r="I81" s="24" t="s">
+      <c r="B81" s="27"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="27"/>
+      <c r="E81" s="27"/>
+      <c r="F81" s="27"/>
+      <c r="G81" s="27"/>
+      <c r="I81" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="J81" s="24"/>
-      <c r="K81" s="24"/>
-      <c r="L81" s="24"/>
-      <c r="M81" s="24"/>
-      <c r="N81" s="24"/>
-      <c r="O81" s="24"/>
+      <c r="J81" s="27"/>
+      <c r="K81" s="27"/>
+      <c r="L81" s="27"/>
+      <c r="M81" s="27"/>
+      <c r="N81" s="27"/>
+      <c r="O81" s="27"/>
     </row>
     <row r="82">
-      <c r="A82" s="27" t="s">
+      <c r="A82" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D82" s="28" t="s">
+      <c r="D82" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="G82" s="44" t="s">
+      <c r="G82" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="I82" s="27" t="s">
+      <c r="I82" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="L82" s="28" t="s">
+      <c r="L82" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="O82" s="45" t="s">
+      <c r="O82" s="46" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="28" t="str">
+      <c r="A83" s="29" t="str">
         <f>CONCATENATE("M 8 ",'Elimination Matches'!G46)</f>
       </c>
-      <c r="B83" s="28"/>
-      <c r="C83" s="28"/>
-      <c r="D83" s="28"/>
-      <c r="E83" s="28"/>
-      <c r="F83" s="28"/>
-      <c r="G83" s="28" t="str">
+      <c r="B83" s="29"/>
+      <c r="C83" s="29"/>
+      <c r="D83" s="29"/>
+      <c r="E83" s="29"/>
+      <c r="F83" s="29"/>
+      <c r="G83" s="29" t="str">
         <f>CONCATENATE("M 9 ",'Elimination Matches'!O46)</f>
       </c>
-      <c r="I83" s="28" t="str">
+      <c r="I83" s="29" t="str">
         <f>CONCATENATE("M 10 ",'Elimination Matches'!G54)</f>
       </c>
-      <c r="J83" s="28"/>
-      <c r="K83" s="28"/>
-      <c r="L83" s="28"/>
-      <c r="M83" s="28"/>
-      <c r="N83" s="28"/>
-      <c r="O83" s="28" t="str">
+      <c r="J83" s="29"/>
+      <c r="K83" s="29"/>
+      <c r="L83" s="29"/>
+      <c r="M83" s="29"/>
+      <c r="N83" s="29"/>
+      <c r="O83" s="29" t="str">
         <f>CONCATENATE("M 11 ",'Elimination Matches'!O54)</f>
       </c>
     </row>
@@ -4069,66 +3827,66 @@
       <c r="O86" s="23"/>
     </row>
     <row r="89">
-      <c r="A89" s="24" t="s">
+      <c r="A89" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="B89" s="24"/>
-      <c r="C89" s="24"/>
-      <c r="D89" s="24"/>
-      <c r="E89" s="24"/>
-      <c r="F89" s="24"/>
-      <c r="G89" s="24"/>
-      <c r="I89" s="24" t="s">
+      <c r="B89" s="27"/>
+      <c r="C89" s="27"/>
+      <c r="D89" s="27"/>
+      <c r="E89" s="27"/>
+      <c r="F89" s="27"/>
+      <c r="G89" s="27"/>
+      <c r="I89" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="J89" s="24"/>
-      <c r="K89" s="24"/>
-      <c r="L89" s="24"/>
-      <c r="M89" s="24"/>
-      <c r="N89" s="24"/>
-      <c r="O89" s="24"/>
+      <c r="J89" s="27"/>
+      <c r="K89" s="27"/>
+      <c r="L89" s="27"/>
+      <c r="M89" s="27"/>
+      <c r="N89" s="27"/>
+      <c r="O89" s="27"/>
     </row>
     <row r="90">
-      <c r="A90" s="27" t="s">
+      <c r="A90" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D90" s="28" t="s">
+      <c r="D90" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="G90" s="46" t="s">
+      <c r="G90" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="I90" s="27" t="s">
+      <c r="I90" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="L90" s="28" t="s">
+      <c r="L90" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="O90" s="47" t="s">
+      <c r="O90" s="48" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="28" t="str">
+      <c r="A91" s="29" t="str">
         <f>CONCATENATE("M 12 ",'Elimination Matches'!G62)</f>
       </c>
-      <c r="B91" s="28"/>
-      <c r="C91" s="28"/>
-      <c r="D91" s="28"/>
-      <c r="E91" s="28"/>
-      <c r="F91" s="28"/>
-      <c r="G91" s="28" t="str">
+      <c r="B91" s="29"/>
+      <c r="C91" s="29"/>
+      <c r="D91" s="29"/>
+      <c r="E91" s="29"/>
+      <c r="F91" s="29"/>
+      <c r="G91" s="29" t="str">
         <f>CONCATENATE("M 13 ",'Elimination Matches'!O62)</f>
       </c>
-      <c r="I91" s="28" t="str">
+      <c r="I91" s="29" t="str">
         <f>CONCATENATE("M 14 ",'Elimination Matches'!G70)</f>
       </c>
-      <c r="J91" s="28"/>
-      <c r="K91" s="28"/>
-      <c r="L91" s="28"/>
-      <c r="M91" s="28"/>
-      <c r="N91" s="28"/>
-      <c r="O91" s="28" t="str">
+      <c r="J91" s="29"/>
+      <c r="K91" s="29"/>
+      <c r="L91" s="29"/>
+      <c r="M91" s="29"/>
+      <c r="N91" s="29"/>
+      <c r="O91" s="29" t="str">
         <f>CONCATENATE("M 15 ",'Elimination Matches'!O70)</f>
       </c>
     </row>
@@ -4153,85 +3911,85 @@
       <c r="O94" s="23"/>
     </row>
     <row r="102">
-      <c r="A102" s="24" t="s">
+      <c r="A102" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="B102" s="24"/>
-      <c r="C102" s="24"/>
-      <c r="D102" s="24"/>
-      <c r="E102" s="24"/>
-      <c r="F102" s="24"/>
-      <c r="G102" s="24"/>
-      <c r="H102" s="24"/>
-      <c r="I102" s="24"/>
-      <c r="J102" s="24"/>
-      <c r="K102" s="24"/>
-      <c r="L102" s="24"/>
-      <c r="M102" s="24"/>
-      <c r="N102" s="24"/>
-      <c r="O102" s="24"/>
+      <c r="B102" s="27"/>
+      <c r="C102" s="27"/>
+      <c r="D102" s="27"/>
+      <c r="E102" s="27"/>
+      <c r="F102" s="27"/>
+      <c r="G102" s="27"/>
+      <c r="H102" s="27"/>
+      <c r="I102" s="27"/>
+      <c r="J102" s="27"/>
+      <c r="K102" s="27"/>
+      <c r="L102" s="27"/>
+      <c r="M102" s="27"/>
+      <c r="N102" s="27"/>
+      <c r="O102" s="27"/>
     </row>
     <row r="104">
-      <c r="A104" s="24" t="s">
+      <c r="A104" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="B104" s="24"/>
-      <c r="C104" s="24"/>
-      <c r="D104" s="24"/>
-      <c r="E104" s="24"/>
-      <c r="F104" s="24"/>
-      <c r="G104" s="24"/>
-      <c r="I104" s="24" t="s">
+      <c r="B104" s="27"/>
+      <c r="C104" s="27"/>
+      <c r="D104" s="27"/>
+      <c r="E104" s="27"/>
+      <c r="F104" s="27"/>
+      <c r="G104" s="27"/>
+      <c r="I104" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="J104" s="24"/>
-      <c r="K104" s="24"/>
-      <c r="L104" s="24"/>
-      <c r="M104" s="24"/>
-      <c r="N104" s="24"/>
-      <c r="O104" s="24"/>
+      <c r="J104" s="27"/>
+      <c r="K104" s="27"/>
+      <c r="L104" s="27"/>
+      <c r="M104" s="27"/>
+      <c r="N104" s="27"/>
+      <c r="O104" s="27"/>
     </row>
     <row r="105">
-      <c r="A105" s="27" t="s">
+      <c r="A105" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D105" s="28" t="s">
+      <c r="D105" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="G105" s="48" t="s">
+      <c r="G105" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="I105" s="27" t="s">
+      <c r="I105" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="L105" s="28" t="s">
+      <c r="L105" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="O105" s="49" t="s">
+      <c r="O105" s="50" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="28" t="str">
+      <c r="A106" s="29" t="str">
         <f>CONCATENATE("M 16 ",'Elimination Matches'!G85)</f>
       </c>
-      <c r="B106" s="28"/>
-      <c r="C106" s="28"/>
-      <c r="D106" s="28"/>
-      <c r="E106" s="28"/>
-      <c r="F106" s="28"/>
-      <c r="G106" s="28" t="str">
+      <c r="B106" s="29"/>
+      <c r="C106" s="29"/>
+      <c r="D106" s="29"/>
+      <c r="E106" s="29"/>
+      <c r="F106" s="29"/>
+      <c r="G106" s="29" t="str">
         <f>CONCATENATE("M 17 ",'Elimination Matches'!O85)</f>
       </c>
-      <c r="I106" s="28" t="str">
+      <c r="I106" s="29" t="str">
         <f>CONCATENATE("M 18 ",'Elimination Matches'!G93)</f>
       </c>
-      <c r="J106" s="28"/>
-      <c r="K106" s="28"/>
-      <c r="L106" s="28"/>
-      <c r="M106" s="28"/>
-      <c r="N106" s="28"/>
-      <c r="O106" s="28" t="str">
+      <c r="J106" s="29"/>
+      <c r="K106" s="29"/>
+      <c r="L106" s="29"/>
+      <c r="M106" s="29"/>
+      <c r="N106" s="29"/>
+      <c r="O106" s="29" t="str">
         <f>CONCATENATE("M 19 ",'Elimination Matches'!O93)</f>
       </c>
     </row>
@@ -4256,56 +4014,56 @@
       <c r="O109" s="23"/>
     </row>
     <row r="117">
-      <c r="A117" s="24" t="s">
+      <c r="A117" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="B117" s="24"/>
-      <c r="C117" s="24"/>
-      <c r="D117" s="24"/>
-      <c r="E117" s="24"/>
-      <c r="F117" s="24"/>
-      <c r="G117" s="24"/>
-      <c r="H117" s="24"/>
-      <c r="I117" s="24"/>
-      <c r="J117" s="24"/>
-      <c r="K117" s="24"/>
-      <c r="L117" s="24"/>
-      <c r="M117" s="24"/>
-      <c r="N117" s="24"/>
-      <c r="O117" s="24"/>
+      <c r="B117" s="27"/>
+      <c r="C117" s="27"/>
+      <c r="D117" s="27"/>
+      <c r="E117" s="27"/>
+      <c r="F117" s="27"/>
+      <c r="G117" s="27"/>
+      <c r="H117" s="27"/>
+      <c r="I117" s="27"/>
+      <c r="J117" s="27"/>
+      <c r="K117" s="27"/>
+      <c r="L117" s="27"/>
+      <c r="M117" s="27"/>
+      <c r="N117" s="27"/>
+      <c r="O117" s="27"/>
     </row>
     <row r="119">
-      <c r="A119" s="24" t="s">
+      <c r="A119" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="B119" s="24"/>
-      <c r="C119" s="24"/>
-      <c r="D119" s="24"/>
-      <c r="E119" s="24"/>
-      <c r="F119" s="24"/>
-      <c r="G119" s="24"/>
+      <c r="B119" s="27"/>
+      <c r="C119" s="27"/>
+      <c r="D119" s="27"/>
+      <c r="E119" s="27"/>
+      <c r="F119" s="27"/>
+      <c r="G119" s="27"/>
     </row>
     <row r="120">
-      <c r="A120" s="27" t="s">
+      <c r="A120" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D120" s="28" t="s">
+      <c r="D120" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="G120" s="50" t="s">
+      <c r="G120" s="51" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="28" t="str">
+      <c r="A121" s="29" t="str">
         <f>CONCATENATE("M 20 ",'Elimination Matches'!G108)</f>
       </c>
-      <c r="B121" s="28"/>
-      <c r="C121" s="28"/>
-      <c r="D121" s="28"/>
-      <c r="E121" s="28"/>
-      <c r="F121" s="28"/>
-      <c r="G121" s="28" t="str">
+      <c r="B121" s="29"/>
+      <c r="C121" s="29"/>
+      <c r="D121" s="29"/>
+      <c r="E121" s="29"/>
+      <c r="F121" s="29"/>
+      <c r="G121" s="29" t="str">
         <f>CONCATENATE("M 21 ",'Elimination Matches'!O108)</f>
       </c>
     </row>

</xml_diff>